<commit_message>
updated LLY, ABBV, AMD
</commit_message>
<xml_diff>
--- a/AMD.xlsx
+++ b/AMD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D214295-CD10-47F6-AE76-733A393A2D02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360875F5-4B46-4FF5-ACD5-095E5708FB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14925" yWindow="2025" windowWidth="29250" windowHeight="18735" activeTab="1" xr2:uid="{449F5976-BBB2-4D6E-9B28-E8B6EC62A528}"/>
+    <workbookView xWindow="3330" yWindow="4590" windowWidth="28110" windowHeight="16515" activeTab="1" xr2:uid="{449F5976-BBB2-4D6E-9B28-E8B6EC62A528}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
   <si>
     <t>Price</t>
   </si>
@@ -145,13 +145,25 @@
   </si>
   <si>
     <t>Revenue y/y</t>
+  </si>
+  <si>
+    <t>Data Center</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Gaming</t>
+  </si>
+  <si>
+    <t>Embedded</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -162,6 +174,13 @@
       <b/>
       <sz val="10"/>
       <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -183,10 +202,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -199,12 +219,28 @@
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{9CDD6D8F-4ABD-4AAD-9484-668CC2275449}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -228,7 +264,7 @@
     <xdr:to>
       <xdr:col>30</xdr:col>
       <xdr:colOff>32657</xdr:colOff>
-      <xdr:row>35</xdr:row>
+      <xdr:row>40</xdr:row>
       <xdr:rowOff>48986</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -246,6 +282,56 @@
         <a:xfrm>
           <a:off x="18641786" y="38100"/>
           <a:ext cx="0" cy="5725886"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>21771</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>54429</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>21771</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>97971</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="4" name="Straight Connector 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{09399797-0FC5-95B2-CB27-D05401A4D136}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9486900" y="54429"/>
+          <a:ext cx="0" cy="4778828"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -560,7 +646,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -643,13 +729,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C865FD-8E44-4C73-A775-FD93E4059E5E}">
-  <dimension ref="A1:AN18"/>
+  <dimension ref="A1:AN25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="T3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="Y3" sqref="Y3"/>
+      <selection pane="bottomRight" activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -660,7 +746,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
     </row>
@@ -791,304 +877,514 @@
         <v>2032</v>
       </c>
     </row>
-    <row r="3" spans="1:40" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="U3" s="6">
-        <v>5299</v>
-      </c>
-      <c r="V3" s="6">
-        <v>5506</v>
-      </c>
-      <c r="W3" s="6">
-        <v>3991</v>
-      </c>
-      <c r="X3" s="6">
-        <v>4272</v>
-      </c>
-      <c r="Y3" s="6">
-        <v>5329</v>
-      </c>
-      <c r="AA3" s="6">
-        <v>6731</v>
-      </c>
-      <c r="AB3" s="6">
-        <v>9763</v>
-      </c>
-      <c r="AC3" s="6">
-        <v>16434</v>
-      </c>
-      <c r="AD3" s="6">
-        <v>23601</v>
+    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" s="10">
+        <v>1293</v>
+      </c>
+      <c r="K3" s="10"/>
+      <c r="L3" s="10"/>
+      <c r="M3" s="10"/>
+      <c r="N3" s="10"/>
+      <c r="O3" s="10">
+        <v>1295</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="AA4" s="3">
-        <v>3863</v>
-      </c>
-      <c r="AB4" s="3">
-        <v>5416</v>
-      </c>
-      <c r="AC4" s="3">
-        <v>8505</v>
-      </c>
-      <c r="AD4" s="3">
-        <v>11550</v>
+        <v>37</v>
+      </c>
+      <c r="J4" s="10">
+        <v>2124</v>
+      </c>
+      <c r="O4" s="2">
+        <v>739</v>
       </c>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>26</v>
-      </c>
-      <c r="AA5" s="3">
-        <f>+AA3-AA4</f>
-        <v>2868</v>
-      </c>
-      <c r="AB5" s="3">
-        <f>+AB3-AB4</f>
-        <v>4347</v>
-      </c>
-      <c r="AC5" s="3">
-        <f>+AC3-AC4</f>
-        <v>7929</v>
-      </c>
-      <c r="AD5" s="3">
-        <f>+AD3-AD4</f>
-        <v>12051</v>
+        <v>38</v>
+      </c>
+      <c r="J5" s="10">
+        <v>1875</v>
+      </c>
+      <c r="K5" s="10"/>
+      <c r="L5" s="10"/>
+      <c r="M5" s="10"/>
+      <c r="N5" s="10"/>
+      <c r="O5" s="10">
+        <v>1757</v>
       </c>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="AA6" s="3">
-        <v>1547</v>
-      </c>
-      <c r="AB6" s="3">
-        <v>1983</v>
-      </c>
-      <c r="AC6" s="3">
-        <v>2845</v>
-      </c>
-      <c r="AD6" s="3">
-        <v>5005</v>
-      </c>
-    </row>
-    <row r="7" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B7" t="s">
-        <v>28</v>
-      </c>
-      <c r="AA7" s="3">
-        <v>750</v>
-      </c>
-      <c r="AB7" s="3">
-        <v>995</v>
-      </c>
-      <c r="AC7" s="3">
-        <v>1448</v>
-      </c>
-      <c r="AD7" s="3">
-        <v>2336</v>
-      </c>
-    </row>
-    <row r="8" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B8" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA8" s="3">
-        <f>+AA6+AA7</f>
-        <v>2297</v>
-      </c>
-      <c r="AB8" s="3">
-        <f>+AB6+AB7</f>
-        <v>2978</v>
-      </c>
-      <c r="AC8" s="3">
-        <f>+AC6+AC7</f>
-        <v>4293</v>
-      </c>
-      <c r="AD8" s="3">
-        <f t="shared" ref="AD8" si="1">+AD6+AD7</f>
-        <v>7341</v>
+        <v>39</v>
+      </c>
+      <c r="J6" s="10">
+        <v>595</v>
+      </c>
+      <c r="K6" s="10"/>
+      <c r="L6" s="10"/>
+      <c r="M6" s="10"/>
+      <c r="N6" s="10"/>
+      <c r="O6" s="10">
+        <v>1562</v>
+      </c>
+    </row>
+    <row r="8" spans="1:40" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="9">
+        <v>5887</v>
+      </c>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
+      <c r="M8" s="9"/>
+      <c r="N8" s="9"/>
+      <c r="O8" s="9">
+        <v>5353</v>
+      </c>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="U8" s="6">
+        <v>5299</v>
+      </c>
+      <c r="V8" s="6">
+        <v>5506</v>
+      </c>
+      <c r="W8" s="6">
+        <v>3991</v>
+      </c>
+      <c r="X8" s="6">
+        <v>4272</v>
+      </c>
+      <c r="Y8" s="6">
+        <v>5329</v>
+      </c>
+      <c r="AA8" s="6">
+        <v>6731</v>
+      </c>
+      <c r="AB8" s="6">
+        <v>9763</v>
+      </c>
+      <c r="AC8" s="6">
+        <v>16434</v>
+      </c>
+      <c r="AD8" s="6">
+        <v>23601</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
-        <v>30</v>
+        <v>25</v>
+      </c>
+      <c r="J9" s="10">
+        <v>2883</v>
+      </c>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10">
+        <v>2689</v>
       </c>
       <c r="AA9" s="3">
-        <f>+AA5-AA8</f>
-        <v>571</v>
+        <v>3863</v>
       </c>
       <c r="AB9" s="3">
-        <f>+AB5-AB8</f>
-        <v>1369</v>
+        <v>5416</v>
       </c>
       <c r="AC9" s="3">
-        <f>+AC5-AC8</f>
-        <v>3636</v>
+        <v>8505</v>
       </c>
       <c r="AD9" s="3">
-        <f t="shared" ref="AD9" si="2">+AD5-AD8</f>
-        <v>4710</v>
+        <v>11550</v>
       </c>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="J10" s="10">
+        <f>J8-J9</f>
+        <v>3004</v>
+      </c>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10">
+        <f>O8-O9</f>
+        <v>2664</v>
+      </c>
+      <c r="AA10" s="3">
+        <f>+AA8-AA9</f>
+        <v>2868</v>
+      </c>
+      <c r="AB10" s="3">
+        <f>+AB8-AB9</f>
+        <v>4347</v>
+      </c>
+      <c r="AC10" s="3">
+        <f>+AC8-AC9</f>
+        <v>7929</v>
+      </c>
+      <c r="AD10" s="3">
+        <f>+AD8-AD9</f>
+        <v>12051</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="10">
+        <v>1060</v>
+      </c>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10">
+        <v>1411</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>1547</v>
+      </c>
+      <c r="AB11" s="3">
+        <v>1983</v>
+      </c>
+      <c r="AC11" s="3">
+        <v>2845</v>
+      </c>
+      <c r="AD11" s="3">
+        <v>5005</v>
+      </c>
+    </row>
+    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="10">
+        <v>597</v>
+      </c>
+      <c r="K12" s="10"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="10"/>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10">
+        <v>585</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>750</v>
+      </c>
+      <c r="AB12" s="3">
+        <v>995</v>
+      </c>
+      <c r="AC12" s="3">
+        <v>1448</v>
+      </c>
+      <c r="AD12" s="3">
+        <v>2336</v>
+      </c>
+    </row>
+    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J13" s="10">
+        <f>J11+J12</f>
+        <v>1657</v>
+      </c>
+      <c r="K13" s="10"/>
+      <c r="L13" s="10"/>
+      <c r="M13" s="10"/>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10">
+        <f>O11+O12</f>
+        <v>1996</v>
+      </c>
+      <c r="AA13" s="3">
+        <f>+AA11+AA12</f>
+        <v>2297</v>
+      </c>
+      <c r="AB13" s="3">
+        <f>+AB11+AB12</f>
+        <v>2978</v>
+      </c>
+      <c r="AC13" s="3">
+        <f>+AC11+AC12</f>
+        <v>4293</v>
+      </c>
+      <c r="AD13" s="3">
+        <f t="shared" ref="AD13" si="1">+AD11+AD12</f>
+        <v>7341</v>
+      </c>
+    </row>
+    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>30</v>
+      </c>
+      <c r="J14" s="10">
+        <f>J10-J13</f>
+        <v>1347</v>
+      </c>
+      <c r="K14" s="10"/>
+      <c r="L14" s="10"/>
+      <c r="M14" s="10"/>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10">
+        <f>O10-O13</f>
+        <v>668</v>
+      </c>
+      <c r="AA14" s="3">
+        <f>+AA10-AA13</f>
+        <v>571</v>
+      </c>
+      <c r="AB14" s="3">
+        <f>+AB10-AB13</f>
+        <v>1369</v>
+      </c>
+      <c r="AC14" s="3">
+        <f>+AC10-AC13</f>
+        <v>3636</v>
+      </c>
+      <c r="AD14" s="3">
+        <f t="shared" ref="AD14" si="2">+AD10-AD13</f>
+        <v>4710</v>
+      </c>
+    </row>
+    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
         <v>31</v>
       </c>
-      <c r="AA10" s="3">
+      <c r="J15" s="10">
+        <f>-13-42</f>
+        <v>-55</v>
+      </c>
+      <c r="K15" s="10"/>
+      <c r="L15" s="10"/>
+      <c r="M15" s="10"/>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10">
+        <f>-25+43</f>
+        <v>18</v>
+      </c>
+      <c r="AA15" s="3">
         <f>-94-165</f>
         <v>-259</v>
       </c>
-      <c r="AB10" s="3">
+      <c r="AB15" s="3">
         <f>-47-47</f>
         <v>-94</v>
       </c>
-      <c r="AC10" s="3">
+      <c r="AC15" s="3">
         <f>-34+55</f>
         <v>21</v>
       </c>
-      <c r="AD10" s="3">
+      <c r="AD15" s="3">
         <f>-88+8</f>
         <v>-80</v>
       </c>
     </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B11" t="s">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="AA11" s="3">
-        <f>+AA9+AA10</f>
+      <c r="J16" s="10">
+        <f>J14+J15</f>
+        <v>1292</v>
+      </c>
+      <c r="K16" s="10"/>
+      <c r="L16" s="10"/>
+      <c r="M16" s="10"/>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10">
+        <f>O14+O15</f>
+        <v>686</v>
+      </c>
+      <c r="AA16" s="3">
+        <f>+AA14+AA15</f>
         <v>312</v>
       </c>
-      <c r="AB11" s="3">
-        <f>+AB9+AB10</f>
+      <c r="AB16" s="3">
+        <f>+AB14+AB15</f>
         <v>1275</v>
       </c>
-      <c r="AC11" s="3">
-        <f>+AC9+AC10</f>
+      <c r="AC16" s="3">
+        <f>+AC14+AC15</f>
         <v>3657</v>
       </c>
-      <c r="AD11" s="3">
-        <f>+AD9+AD10</f>
+      <c r="AD16" s="3">
+        <f>+AD14+AD15</f>
         <v>4630</v>
       </c>
     </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B12" t="s">
+    <row r="17" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
         <v>33</v>
       </c>
-      <c r="AA12" s="3">
+      <c r="J17" s="10">
+        <v>113</v>
+      </c>
+      <c r="K17" s="10"/>
+      <c r="L17" s="10"/>
+      <c r="M17" s="10"/>
+      <c r="N17" s="10"/>
+      <c r="O17" s="10">
+        <v>13</v>
+      </c>
+      <c r="AA17" s="3">
         <v>0</v>
       </c>
-      <c r="AB12" s="3">
+      <c r="AB17" s="3">
         <v>0</v>
       </c>
-      <c r="AC12" s="3">
+      <c r="AC17" s="3">
         <v>513</v>
       </c>
-      <c r="AD12" s="3">
+      <c r="AD17" s="3">
         <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B13" t="s">
-        <v>34</v>
-      </c>
-      <c r="AA13" s="3">
-        <f>+AA11-AA12</f>
-        <v>312</v>
-      </c>
-      <c r="AB13" s="3">
-        <f>+AB11-AB12</f>
-        <v>1275</v>
-      </c>
-      <c r="AC13" s="3">
-        <f>+AC11-AC12</f>
-        <v>3144</v>
-      </c>
-      <c r="AD13" s="3">
-        <f>+AD11-AD12</f>
-        <v>4630</v>
-      </c>
-    </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
-        <v>24</v>
-      </c>
-      <c r="AA14" s="1">
-        <f>+AA13/AA15</f>
-        <v>0.27857142857142858</v>
-      </c>
-      <c r="AB14" s="1">
-        <f>+AB13/AB15</f>
-        <v>1.056338028169014</v>
-      </c>
-      <c r="AC14" s="1">
-        <f>+AC13/AC15</f>
-        <v>2.5581773799837264</v>
-      </c>
-      <c r="AD14" s="1">
-        <f>+AD13/AD15</f>
-        <v>2.9471674092934435</v>
-      </c>
-    </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA15" s="3">
-        <v>1120</v>
-      </c>
-      <c r="AB15" s="3">
-        <v>1207</v>
-      </c>
-      <c r="AC15" s="3">
-        <v>1229</v>
-      </c>
-      <c r="AD15" s="3">
-        <v>1571</v>
       </c>
     </row>
     <row r="18" spans="2:30" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
+        <v>34</v>
+      </c>
+      <c r="J18" s="10">
+        <f>J16-J17</f>
+        <v>1179</v>
+      </c>
+      <c r="K18" s="10"/>
+      <c r="L18" s="10"/>
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="10">
+        <f>O16-O17</f>
+        <v>673</v>
+      </c>
+      <c r="AA18" s="3">
+        <f>+AA16-AA17</f>
+        <v>312</v>
+      </c>
+      <c r="AB18" s="3">
+        <f>+AB16-AB17</f>
+        <v>1275</v>
+      </c>
+      <c r="AC18" s="3">
+        <f>+AC16-AC17</f>
+        <v>3144</v>
+      </c>
+      <c r="AD18" s="3">
+        <f>+AD16-AD17</f>
+        <v>4630</v>
+      </c>
+    </row>
+    <row r="19" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>24</v>
+      </c>
+      <c r="J19" s="11">
+        <f>J18/J20</f>
+        <v>0.83617021276595749</v>
+      </c>
+      <c r="O19" s="11">
+        <f>O18/O20</f>
+        <v>0.41775294847920547</v>
+      </c>
+      <c r="AA19" s="1">
+        <f>+AA18/AA20</f>
+        <v>0.27857142857142858</v>
+      </c>
+      <c r="AB19" s="1">
+        <f>+AB18/AB20</f>
+        <v>1.056338028169014</v>
+      </c>
+      <c r="AC19" s="1">
+        <f>+AC18/AC20</f>
+        <v>2.5581773799837264</v>
+      </c>
+      <c r="AD19" s="1">
+        <f>+AD18/AD20</f>
+        <v>2.9471674092934435</v>
+      </c>
+    </row>
+    <row r="20" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>1</v>
+      </c>
+      <c r="J20" s="10">
+        <v>1410</v>
+      </c>
+      <c r="K20" s="10"/>
+      <c r="L20" s="10"/>
+      <c r="M20" s="10"/>
+      <c r="N20" s="10"/>
+      <c r="O20" s="10">
+        <v>1611</v>
+      </c>
+      <c r="AA20" s="3">
+        <v>1120</v>
+      </c>
+      <c r="AB20" s="3">
+        <v>1207</v>
+      </c>
+      <c r="AC20" s="3">
+        <v>1229</v>
+      </c>
+      <c r="AD20" s="3">
+        <v>1571</v>
+      </c>
+    </row>
+    <row r="23" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
         <v>35</v>
       </c>
-      <c r="AB18" s="7">
-        <f>+AB3/AA3-1</f>
+      <c r="O23" s="12">
+        <f>O8/J8-1</f>
+        <v>-9.0708340411075228E-2</v>
+      </c>
+      <c r="AB23" s="7">
+        <f>+AB8/AA8-1</f>
         <v>0.45045312732134901</v>
       </c>
-      <c r="AC18" s="7">
-        <f>+AC3/AB3-1</f>
+      <c r="AC23" s="7">
+        <f>+AC8/AB8-1</f>
         <v>0.68329406944586712</v>
       </c>
-      <c r="AD18" s="7">
-        <f>+AD3/AC3-1</f>
+      <c r="AD23" s="7">
+        <f>+AD8/AC8-1</f>
         <v>0.43610806863818907</v>
       </c>
     </row>
+    <row r="25" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="B25" t="s">
+        <v>26</v>
+      </c>
+      <c r="J25" s="12">
+        <f>J10/J8</f>
+        <v>0.51027688126380155</v>
+      </c>
+      <c r="O25" s="12">
+        <f>O10/O8</f>
+        <v>0.49766486082570521</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="Main!A1" display="Main" xr:uid="{AE73617B-F45B-445A-BDA8-AE857C9E0C10}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updated INTC AMD models
</commit_message>
<xml_diff>
--- a/AMD.xlsx
+++ b/AMD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{360875F5-4B46-4FF5-ACD5-095E5708FB9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{695AD5D5-5B73-4EFB-9063-AF17170A6DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3330" yWindow="4590" windowWidth="28110" windowHeight="16515" activeTab="1" xr2:uid="{449F5976-BBB2-4D6E-9B28-E8B6EC62A528}"/>
+    <workbookView xWindow="-23925" yWindow="915" windowWidth="23250" windowHeight="18870" activeTab="1" xr2:uid="{449F5976-BBB2-4D6E-9B28-E8B6EC62A528}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="44">
   <si>
     <t>Price</t>
   </si>
@@ -157,6 +157,18 @@
   </si>
   <si>
     <t>Embedded</t>
+  </si>
+  <si>
+    <t>Q124</t>
+  </si>
+  <si>
+    <t>Q224</t>
+  </si>
+  <si>
+    <t>Q324</t>
+  </si>
+  <si>
+    <t>Q424</t>
   </si>
 </sst>
 </file>
@@ -256,16 +268,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>32657</xdr:colOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>48986</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
-      <xdr:colOff>32657</xdr:colOff>
+      <xdr:col>36</xdr:col>
+      <xdr:colOff>48986</xdr:colOff>
       <xdr:row>40</xdr:row>
-      <xdr:rowOff>48986</xdr:rowOff>
+      <xdr:rowOff>10886</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -280,8 +292,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="18641786" y="38100"/>
-          <a:ext cx="0" cy="5725886"/>
+          <a:off x="22315715" y="0"/>
+          <a:ext cx="0" cy="6542315"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -306,16 +318,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>21771</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>54429</xdr:rowOff>
+      <xdr:rowOff>21771</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
+      <xdr:col>20</xdr:col>
       <xdr:colOff>21771</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>97971</xdr:rowOff>
+      <xdr:rowOff>65313</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -330,7 +342,7 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9486900" y="54429"/>
+          <a:off x="12534900" y="21771"/>
           <a:ext cx="0" cy="4778828"/>
         </a:xfrm>
         <a:prstGeom prst="line">
@@ -358,9 +370,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -398,7 +410,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -504,7 +516,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -646,7 +658,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -729,28 +741,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C865FD-8E44-4C73-A775-FD93E4059E5E}">
-  <dimension ref="A1:AN25"/>
+  <dimension ref="A1:AS25"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="AC3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="O20" sqref="O20"/>
+      <selection pane="bottomRight" activeCell="AH3" sqref="AH3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="18" width="9.140625" style="2"/>
+    <col min="3" max="23" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
@@ -799,141 +811,218 @@
       <c r="R2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="U2">
+      <c r="S2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z2">
         <v>2013</v>
       </c>
-      <c r="V2">
+      <c r="AA2">
         <v>2014</v>
       </c>
-      <c r="W2">
+      <c r="AB2">
         <v>2015</v>
       </c>
-      <c r="X2">
-        <f>+W2+1</f>
+      <c r="AC2">
+        <f>+AB2+1</f>
         <v>2016</v>
       </c>
-      <c r="Y2">
-        <f t="shared" ref="Y2:AN2" si="0">+X2+1</f>
+      <c r="AD2">
+        <f t="shared" ref="AD2:AS2" si="0">+AC2+1</f>
         <v>2017</v>
       </c>
-      <c r="Z2">
+      <c r="AE2">
         <f t="shared" si="0"/>
         <v>2018</v>
       </c>
-      <c r="AA2">
+      <c r="AF2">
         <f t="shared" si="0"/>
         <v>2019</v>
       </c>
-      <c r="AB2">
+      <c r="AG2">
         <f t="shared" si="0"/>
         <v>2020</v>
       </c>
-      <c r="AC2">
+      <c r="AH2">
         <f t="shared" si="0"/>
         <v>2021</v>
       </c>
-      <c r="AD2">
+      <c r="AI2">
         <f t="shared" si="0"/>
         <v>2022</v>
       </c>
-      <c r="AE2">
+      <c r="AJ2">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="AF2">
+      <c r="AK2">
         <f t="shared" si="0"/>
         <v>2024</v>
       </c>
-      <c r="AG2">
+      <c r="AL2">
         <f t="shared" si="0"/>
         <v>2025</v>
       </c>
-      <c r="AH2">
+      <c r="AM2">
         <f t="shared" si="0"/>
         <v>2026</v>
       </c>
-      <c r="AI2">
+      <c r="AN2">
         <f t="shared" si="0"/>
         <v>2027</v>
       </c>
-      <c r="AJ2">
+      <c r="AO2">
         <f t="shared" si="0"/>
         <v>2028</v>
       </c>
-      <c r="AK2">
+      <c r="AP2">
         <f t="shared" si="0"/>
         <v>2029</v>
       </c>
-      <c r="AL2">
+      <c r="AQ2">
         <f t="shared" si="0"/>
         <v>2030</v>
       </c>
-      <c r="AM2">
+      <c r="AR2">
         <f t="shared" si="0"/>
         <v>2031</v>
       </c>
-      <c r="AN2">
+      <c r="AS2">
         <f t="shared" si="0"/>
         <v>2032</v>
       </c>
     </row>
-    <row r="3" spans="1:40" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>36</v>
       </c>
-      <c r="J3" s="10">
+      <c r="J3" s="10"/>
+      <c r="K3" s="10">
         <v>1293</v>
       </c>
-      <c r="K3" s="10"/>
       <c r="L3" s="10"/>
       <c r="M3" s="10"/>
       <c r="N3" s="10"/>
       <c r="O3" s="10">
         <v>1295</v>
       </c>
-    </row>
-    <row r="4" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="P3" s="10">
+        <v>1321</v>
+      </c>
+      <c r="Q3" s="10"/>
+      <c r="R3" s="10"/>
+      <c r="S3" s="10"/>
+      <c r="T3" s="10">
+        <v>2834</v>
+      </c>
+      <c r="AI3" s="3">
+        <v>6043</v>
+      </c>
+      <c r="AJ3" s="3">
+        <v>6496</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="10">
+      <c r="J4" s="10"/>
+      <c r="K4" s="10">
         <v>2124</v>
       </c>
       <c r="O4" s="2">
         <v>739</v>
       </c>
-    </row>
-    <row r="5" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="P4" s="10">
+        <v>998</v>
+      </c>
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10">
+        <v>1492</v>
+      </c>
+      <c r="AI4" s="3">
+        <v>6201</v>
+      </c>
+      <c r="AJ4" s="3">
+        <v>4651</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>38</v>
       </c>
-      <c r="J5" s="10">
+      <c r="J5" s="10"/>
+      <c r="K5" s="10">
         <v>1875</v>
       </c>
-      <c r="K5" s="10"/>
       <c r="L5" s="10"/>
       <c r="M5" s="10"/>
       <c r="N5" s="10"/>
       <c r="O5" s="10">
         <v>1757</v>
       </c>
-    </row>
-    <row r="6" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="P5" s="10">
+        <v>1581</v>
+      </c>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="10"/>
+      <c r="S5" s="10"/>
+      <c r="T5" s="10">
+        <v>648</v>
+      </c>
+      <c r="AI5" s="3">
+        <v>6805</v>
+      </c>
+      <c r="AJ5" s="3">
+        <v>6212</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>39</v>
       </c>
-      <c r="J6" s="10">
+      <c r="J6" s="10"/>
+      <c r="K6" s="10">
         <v>595</v>
       </c>
-      <c r="K6" s="10"/>
       <c r="L6" s="10"/>
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
       <c r="O6" s="10">
         <v>1562</v>
       </c>
-    </row>
-    <row r="8" spans="1:40" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="P6" s="10">
+        <v>1459</v>
+      </c>
+      <c r="Q6" s="10"/>
+      <c r="R6" s="10"/>
+      <c r="S6" s="10"/>
+      <c r="T6" s="10">
+        <v>861</v>
+      </c>
+      <c r="AI6" s="3">
+        <v>4552</v>
+      </c>
+      <c r="AJ6" s="3">
+        <v>5321</v>
+      </c>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AI7" s="3"/>
+      <c r="AJ7" s="3"/>
+    </row>
+    <row r="8" spans="1:45" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
@@ -944,441 +1033,1026 @@
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
-      <c r="J8" s="9">
+      <c r="J8" s="9"/>
+      <c r="K8" s="9">
         <v>5887</v>
       </c>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="M8" s="9"/>
-      <c r="N8" s="9"/>
+      <c r="L8" s="9">
+        <v>6550</v>
+      </c>
+      <c r="M8" s="9">
+        <v>5565</v>
+      </c>
+      <c r="N8" s="9">
+        <f>+AI8-M8-L8-K8</f>
+        <v>5599</v>
+      </c>
       <c r="O8" s="9">
         <v>5353</v>
       </c>
-      <c r="P8" s="5"/>
-      <c r="Q8" s="5"/>
-      <c r="R8" s="5"/>
-      <c r="U8" s="6">
+      <c r="P8" s="9">
+        <v>5359</v>
+      </c>
+      <c r="Q8" s="9">
+        <v>5800</v>
+      </c>
+      <c r="R8" s="9">
+        <f>+AJ8-Q8-P8-O8</f>
+        <v>6168</v>
+      </c>
+      <c r="S8" s="9">
+        <v>5473</v>
+      </c>
+      <c r="T8" s="9">
+        <v>5835</v>
+      </c>
+      <c r="U8" s="5"/>
+      <c r="V8" s="5"/>
+      <c r="W8" s="5"/>
+      <c r="Z8" s="6">
         <v>5299</v>
       </c>
-      <c r="V8" s="6">
+      <c r="AA8" s="6">
         <v>5506</v>
       </c>
-      <c r="W8" s="6">
+      <c r="AB8" s="6">
         <v>3991</v>
       </c>
-      <c r="X8" s="6">
+      <c r="AC8" s="6">
         <v>4272</v>
       </c>
-      <c r="Y8" s="6">
+      <c r="AD8" s="6">
         <v>5329</v>
       </c>
-      <c r="AA8" s="6">
+      <c r="AE8" s="6">
+        <v>6475</v>
+      </c>
+      <c r="AF8" s="6">
         <v>6731</v>
       </c>
-      <c r="AB8" s="6">
+      <c r="AG8" s="6">
         <v>9763</v>
       </c>
-      <c r="AC8" s="6">
+      <c r="AH8" s="6">
         <v>16434</v>
       </c>
-      <c r="AD8" s="6">
+      <c r="AI8" s="6">
         <v>23601</v>
       </c>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AJ8" s="6">
+        <f>SUM(AJ3:AJ6)</f>
+        <v>22680</v>
+      </c>
+    </row>
+    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="J9" s="10">
+      <c r="J9" s="10"/>
+      <c r="K9" s="10">
         <v>2883</v>
       </c>
-      <c r="K9" s="10"/>
-      <c r="L9" s="10"/>
-      <c r="M9" s="10"/>
-      <c r="N9" s="10"/>
+      <c r="L9" s="10">
+        <v>3115</v>
+      </c>
+      <c r="M9" s="10">
+        <v>2799</v>
+      </c>
+      <c r="N9" s="10">
+        <f>+AI9-M9-L9-K9</f>
+        <v>2753</v>
+      </c>
       <c r="O9" s="10">
         <v>2689</v>
       </c>
-      <c r="AA9" s="3">
+      <c r="P9" s="10">
+        <v>2704</v>
+      </c>
+      <c r="Q9" s="10">
+        <v>2843</v>
+      </c>
+      <c r="R9" s="10">
+        <f>+AJ9-Q9-P9-O9</f>
+        <v>3042</v>
+      </c>
+      <c r="S9" s="10">
+        <v>2683</v>
+      </c>
+      <c r="T9" s="10">
+        <v>2740</v>
+      </c>
+      <c r="AD9" s="3">
+        <v>3466</v>
+      </c>
+      <c r="AE9" s="3">
+        <v>4028</v>
+      </c>
+      <c r="AF9" s="3">
         <v>3863</v>
       </c>
-      <c r="AB9" s="3">
+      <c r="AG9" s="3">
         <v>5416</v>
       </c>
-      <c r="AC9" s="3">
+      <c r="AH9" s="3">
         <v>8505</v>
       </c>
-      <c r="AD9" s="3">
+      <c r="AI9" s="3">
         <v>11550</v>
       </c>
-    </row>
-    <row r="10" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AJ9" s="3">
+        <v>11278</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>26</v>
       </c>
-      <c r="J10" s="10">
-        <f>J8-J9</f>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10">
+        <f>K8-K9</f>
         <v>3004</v>
       </c>
-      <c r="K10" s="10"/>
-      <c r="L10" s="10"/>
-      <c r="M10" s="10"/>
-      <c r="N10" s="10"/>
+      <c r="L10" s="10">
+        <f>L8-L9</f>
+        <v>3435</v>
+      </c>
+      <c r="M10" s="10">
+        <f>M8-M9</f>
+        <v>2766</v>
+      </c>
+      <c r="N10" s="10">
+        <f>+N8-N9</f>
+        <v>2846</v>
+      </c>
       <c r="O10" s="10">
-        <f>O8-O9</f>
+        <f t="shared" ref="O10:T10" si="1">O8-O9</f>
         <v>2664</v>
       </c>
-      <c r="AA10" s="3">
-        <f>+AA8-AA9</f>
+      <c r="P10" s="10">
+        <f t="shared" si="1"/>
+        <v>2655</v>
+      </c>
+      <c r="Q10" s="10">
+        <f t="shared" si="1"/>
+        <v>2957</v>
+      </c>
+      <c r="R10" s="10">
+        <f t="shared" si="1"/>
+        <v>3126</v>
+      </c>
+      <c r="S10" s="10">
+        <f t="shared" si="1"/>
+        <v>2790</v>
+      </c>
+      <c r="T10" s="10">
+        <f t="shared" si="1"/>
+        <v>3095</v>
+      </c>
+      <c r="AD10" s="3">
+        <f t="shared" ref="AD10:AJ10" si="2">+AD8-AD9</f>
+        <v>1863</v>
+      </c>
+      <c r="AE10" s="3">
+        <f t="shared" si="2"/>
+        <v>2447</v>
+      </c>
+      <c r="AF10" s="3">
+        <f t="shared" si="2"/>
         <v>2868</v>
       </c>
-      <c r="AB10" s="3">
-        <f>+AB8-AB9</f>
+      <c r="AG10" s="3">
+        <f t="shared" si="2"/>
         <v>4347</v>
       </c>
-      <c r="AC10" s="3">
-        <f>+AC8-AC9</f>
+      <c r="AH10" s="3">
+        <f t="shared" si="2"/>
         <v>7929</v>
       </c>
-      <c r="AD10" s="3">
-        <f>+AD8-AD9</f>
+      <c r="AI10" s="3">
+        <f t="shared" si="2"/>
         <v>12051</v>
       </c>
-    </row>
-    <row r="11" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AJ10" s="3">
+        <f t="shared" si="2"/>
+        <v>11402</v>
+      </c>
+    </row>
+    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>27</v>
       </c>
-      <c r="J11" s="10">
+      <c r="J11" s="10"/>
+      <c r="K11" s="10">
         <v>1060</v>
       </c>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
+      <c r="L11" s="10">
+        <v>1300</v>
+      </c>
+      <c r="M11" s="10">
+        <v>1279</v>
+      </c>
+      <c r="N11" s="10">
+        <f t="shared" ref="N11:N12" si="3">+AI11-M11-L11-K11</f>
+        <v>1366</v>
+      </c>
       <c r="O11" s="10">
         <v>1411</v>
       </c>
-      <c r="AA11" s="3">
+      <c r="P11" s="10">
+        <v>1443</v>
+      </c>
+      <c r="Q11" s="10">
+        <v>1507</v>
+      </c>
+      <c r="R11" s="10">
+        <f>+AJ11-Q11-P11-O11</f>
+        <v>1511</v>
+      </c>
+      <c r="S11" s="10">
+        <v>1525</v>
+      </c>
+      <c r="T11" s="10">
+        <v>1583</v>
+      </c>
+      <c r="AD11" s="3">
+        <v>1196</v>
+      </c>
+      <c r="AE11" s="3">
+        <v>1434</v>
+      </c>
+      <c r="AF11" s="3">
         <v>1547</v>
       </c>
-      <c r="AB11" s="3">
+      <c r="AG11" s="3">
         <v>1983</v>
       </c>
-      <c r="AC11" s="3">
+      <c r="AH11" s="3">
         <v>2845</v>
       </c>
-      <c r="AD11" s="3">
+      <c r="AI11" s="3">
         <v>5005</v>
       </c>
-    </row>
-    <row r="12" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AJ11" s="3">
+        <v>5872</v>
+      </c>
+    </row>
+    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="10">
+      <c r="J12" s="10"/>
+      <c r="K12" s="10">
         <v>597</v>
       </c>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
+      <c r="L12" s="10">
+        <v>592</v>
+      </c>
+      <c r="M12" s="10">
+        <v>557</v>
+      </c>
+      <c r="N12" s="10">
+        <f t="shared" si="3"/>
+        <v>590</v>
+      </c>
       <c r="O12" s="10">
         <v>585</v>
       </c>
-      <c r="AA12" s="3">
+      <c r="P12" s="10">
+        <v>547</v>
+      </c>
+      <c r="Q12" s="10">
+        <v>576</v>
+      </c>
+      <c r="R12" s="10">
+        <f>+AJ12-Q12-P12-O12</f>
+        <v>644</v>
+      </c>
+      <c r="S12" s="10">
+        <v>620</v>
+      </c>
+      <c r="T12" s="10">
+        <v>650</v>
+      </c>
+      <c r="AD12" s="3">
+        <v>516</v>
+      </c>
+      <c r="AE12" s="3">
+        <v>562</v>
+      </c>
+      <c r="AF12" s="3">
         <v>750</v>
       </c>
-      <c r="AB12" s="3">
+      <c r="AG12" s="3">
         <v>995</v>
       </c>
-      <c r="AC12" s="3">
+      <c r="AH12" s="3">
         <v>1448</v>
       </c>
-      <c r="AD12" s="3">
+      <c r="AI12" s="3">
         <v>2336</v>
       </c>
-    </row>
-    <row r="13" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AJ12" s="3">
+        <v>2352</v>
+      </c>
+    </row>
+    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>29</v>
       </c>
-      <c r="J13" s="10">
-        <f>J11+J12</f>
+      <c r="J13" s="10"/>
+      <c r="K13" s="10">
+        <f>K11+K12</f>
         <v>1657</v>
       </c>
-      <c r="K13" s="10"/>
-      <c r="L13" s="10"/>
-      <c r="M13" s="10"/>
-      <c r="N13" s="10"/>
+      <c r="L13" s="10">
+        <f>L11+L12</f>
+        <v>1892</v>
+      </c>
+      <c r="M13" s="10">
+        <f>M11+M12</f>
+        <v>1836</v>
+      </c>
+      <c r="N13" s="10">
+        <f t="shared" ref="N13" si="4">N11+N12</f>
+        <v>1956</v>
+      </c>
       <c r="O13" s="10">
-        <f>O11+O12</f>
+        <f t="shared" ref="O13:T13" si="5">O11+O12</f>
         <v>1996</v>
       </c>
-      <c r="AA13" s="3">
-        <f>+AA11+AA12</f>
+      <c r="P13" s="10">
+        <f t="shared" si="5"/>
+        <v>1990</v>
+      </c>
+      <c r="Q13" s="10">
+        <f t="shared" si="5"/>
+        <v>2083</v>
+      </c>
+      <c r="R13" s="10">
+        <f t="shared" si="5"/>
+        <v>2155</v>
+      </c>
+      <c r="S13" s="10">
+        <f t="shared" si="5"/>
+        <v>2145</v>
+      </c>
+      <c r="T13" s="10">
+        <f t="shared" si="5"/>
+        <v>2233</v>
+      </c>
+      <c r="AD13" s="3">
+        <f>+AD11+AD12</f>
+        <v>1712</v>
+      </c>
+      <c r="AE13" s="3">
+        <f>+AE11+AE12</f>
+        <v>1996</v>
+      </c>
+      <c r="AF13" s="3">
+        <f>+AF11+AF12</f>
         <v>2297</v>
       </c>
-      <c r="AB13" s="3">
-        <f>+AB11+AB12</f>
+      <c r="AG13" s="3">
+        <f>+AG11+AG12</f>
         <v>2978</v>
       </c>
-      <c r="AC13" s="3">
-        <f>+AC11+AC12</f>
+      <c r="AH13" s="3">
+        <f>+AH11+AH12</f>
         <v>4293</v>
       </c>
-      <c r="AD13" s="3">
-        <f t="shared" ref="AD13" si="1">+AD11+AD12</f>
+      <c r="AI13" s="3">
+        <f t="shared" ref="AI13:AJ13" si="6">+AI11+AI12</f>
         <v>7341</v>
       </c>
-    </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AJ13" s="3">
+        <f t="shared" si="6"/>
+        <v>8224</v>
+      </c>
+    </row>
+    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>30</v>
       </c>
-      <c r="J14" s="10">
-        <f>J10-J13</f>
+      <c r="J14" s="10"/>
+      <c r="K14" s="10">
+        <f>K10-K13</f>
         <v>1347</v>
       </c>
-      <c r="K14" s="10"/>
-      <c r="L14" s="10"/>
-      <c r="M14" s="10"/>
-      <c r="N14" s="10"/>
+      <c r="L14" s="10">
+        <f>L10-L13</f>
+        <v>1543</v>
+      </c>
+      <c r="M14" s="10">
+        <f>M10-M13</f>
+        <v>930</v>
+      </c>
+      <c r="N14" s="10">
+        <f t="shared" ref="N14" si="7">N10-N13</f>
+        <v>890</v>
+      </c>
       <c r="O14" s="10">
-        <f>O10-O13</f>
+        <f t="shared" ref="O14:T14" si="8">O10-O13</f>
         <v>668</v>
       </c>
-      <c r="AA14" s="3">
-        <f>+AA10-AA13</f>
+      <c r="P14" s="10">
+        <f t="shared" si="8"/>
+        <v>665</v>
+      </c>
+      <c r="Q14" s="10">
+        <f t="shared" si="8"/>
+        <v>874</v>
+      </c>
+      <c r="R14" s="10">
+        <f t="shared" si="8"/>
+        <v>971</v>
+      </c>
+      <c r="S14" s="10">
+        <f t="shared" si="8"/>
+        <v>645</v>
+      </c>
+      <c r="T14" s="10">
+        <f t="shared" si="8"/>
+        <v>862</v>
+      </c>
+      <c r="AD14" s="3">
+        <f>+AD10-AD13</f>
+        <v>151</v>
+      </c>
+      <c r="AE14" s="3">
+        <f>+AE10-AE13</f>
+        <v>451</v>
+      </c>
+      <c r="AF14" s="3">
+        <f>+AF10-AF13</f>
         <v>571</v>
       </c>
-      <c r="AB14" s="3">
-        <f>+AB10-AB13</f>
+      <c r="AG14" s="3">
+        <f>+AG10-AG13</f>
         <v>1369</v>
       </c>
-      <c r="AC14" s="3">
-        <f>+AC10-AC13</f>
+      <c r="AH14" s="3">
+        <f>+AH10-AH13</f>
         <v>3636</v>
       </c>
-      <c r="AD14" s="3">
-        <f t="shared" ref="AD14" si="2">+AD10-AD13</f>
+      <c r="AI14" s="3">
+        <f t="shared" ref="AI14:AJ14" si="9">+AI10-AI13</f>
         <v>4710</v>
       </c>
-    </row>
-    <row r="15" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AJ14" s="3">
+        <f t="shared" si="9"/>
+        <v>3178</v>
+      </c>
+    </row>
+    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>31</v>
       </c>
-      <c r="J15" s="10">
+      <c r="J15" s="10"/>
+      <c r="K15" s="10">
         <f>-13-42</f>
         <v>-55</v>
       </c>
-      <c r="K15" s="10"/>
-      <c r="L15" s="10"/>
-      <c r="M15" s="10"/>
+      <c r="L15" s="10">
+        <f>-25-4</f>
+        <v>-29</v>
+      </c>
+      <c r="M15" s="10">
+        <f>-25+43</f>
+        <v>18</v>
+      </c>
       <c r="N15" s="10"/>
       <c r="O15" s="10">
         <f>-25+43</f>
         <v>18</v>
       </c>
-      <c r="AA15" s="3">
+      <c r="P15" s="10">
+        <f>-28+46</f>
+        <v>18</v>
+      </c>
+      <c r="Q15" s="10">
+        <f>-26+59</f>
+        <v>33</v>
+      </c>
+      <c r="R15" s="10">
+        <f>+AJ15-Q15-P15-O15</f>
+        <v>22</v>
+      </c>
+      <c r="S15" s="10">
+        <f>-25+53</f>
+        <v>28</v>
+      </c>
+      <c r="T15" s="10">
+        <f>-25+55</f>
+        <v>30</v>
+      </c>
+      <c r="AD15" s="3">
+        <v>-121</v>
+      </c>
+      <c r="AE15" s="3">
+        <v>-121</v>
+      </c>
+      <c r="AF15" s="3">
         <f>-94-165</f>
         <v>-259</v>
       </c>
-      <c r="AB15" s="3">
+      <c r="AG15" s="3">
         <f>-47-47</f>
         <v>-94</v>
       </c>
-      <c r="AC15" s="3">
+      <c r="AH15" s="3">
         <f>-34+55</f>
         <v>21</v>
       </c>
-      <c r="AD15" s="3">
+      <c r="AI15" s="3">
         <f>-88+8</f>
         <v>-80</v>
       </c>
-    </row>
-    <row r="16" spans="1:40" x14ac:dyDescent="0.2">
+      <c r="AJ15">
+        <f>-106+197</f>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>32</v>
       </c>
-      <c r="J16" s="10">
-        <f>J14+J15</f>
+      <c r="J16" s="10"/>
+      <c r="K16" s="10">
+        <f>K14+K15</f>
         <v>1292</v>
       </c>
-      <c r="K16" s="10"/>
-      <c r="L16" s="10"/>
-      <c r="M16" s="10"/>
-      <c r="N16" s="10"/>
+      <c r="L16" s="10">
+        <f>L14+L15</f>
+        <v>1514</v>
+      </c>
+      <c r="M16" s="10">
+        <f>M14+M15</f>
+        <v>948</v>
+      </c>
+      <c r="N16" s="10">
+        <f t="shared" ref="N16" si="10">N14+N15</f>
+        <v>890</v>
+      </c>
       <c r="O16" s="10">
-        <f>O14+O15</f>
+        <f t="shared" ref="O16:T16" si="11">O14+O15</f>
         <v>686</v>
       </c>
-      <c r="AA16" s="3">
-        <f>+AA14+AA15</f>
+      <c r="P16" s="10">
+        <f t="shared" si="11"/>
+        <v>683</v>
+      </c>
+      <c r="Q16" s="10">
+        <f t="shared" si="11"/>
+        <v>907</v>
+      </c>
+      <c r="R16" s="10">
+        <f t="shared" si="11"/>
+        <v>993</v>
+      </c>
+      <c r="S16" s="10">
+        <f t="shared" si="11"/>
+        <v>673</v>
+      </c>
+      <c r="T16" s="10">
+        <f t="shared" si="11"/>
+        <v>892</v>
+      </c>
+      <c r="AD16" s="3">
+        <f t="shared" ref="AD16:AJ16" si="12">+AD14+AD15</f>
+        <v>30</v>
+      </c>
+      <c r="AE16" s="3">
+        <f t="shared" si="12"/>
+        <v>330</v>
+      </c>
+      <c r="AF16" s="3">
+        <f t="shared" si="12"/>
         <v>312</v>
       </c>
-      <c r="AB16" s="3">
-        <f>+AB14+AB15</f>
+      <c r="AG16" s="3">
+        <f t="shared" si="12"/>
         <v>1275</v>
       </c>
-      <c r="AC16" s="3">
-        <f>+AC14+AC15</f>
+      <c r="AH16" s="3">
+        <f t="shared" si="12"/>
         <v>3657</v>
       </c>
-      <c r="AD16" s="3">
-        <f>+AD14+AD15</f>
+      <c r="AI16" s="3">
+        <f t="shared" si="12"/>
         <v>4630</v>
       </c>
-    </row>
-    <row r="17" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="AJ16" s="3">
+        <f t="shared" si="12"/>
+        <v>3269</v>
+      </c>
+    </row>
+    <row r="17" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>33</v>
       </c>
-      <c r="J17" s="10">
+      <c r="J17" s="10"/>
+      <c r="K17" s="10">
         <v>113</v>
       </c>
-      <c r="K17" s="10"/>
-      <c r="L17" s="10"/>
-      <c r="M17" s="10"/>
+      <c r="L17" s="10">
+        <v>54</v>
+      </c>
+      <c r="M17" s="10">
+        <v>13</v>
+      </c>
       <c r="N17" s="10"/>
       <c r="O17" s="10">
         <v>13</v>
       </c>
-      <c r="AA17" s="3">
+      <c r="P17" s="10">
+        <v>-23</v>
+      </c>
+      <c r="Q17" s="10">
+        <v>-39</v>
+      </c>
+      <c r="R17" s="10">
+        <f>+AJ17-Q17-P17-O17</f>
+        <v>395</v>
+      </c>
+      <c r="S17" s="10">
+        <v>52</v>
+      </c>
+      <c r="T17" s="10">
+        <v>41</v>
+      </c>
+      <c r="AD17" s="3">
+        <f>9+2</f>
+        <v>11</v>
+      </c>
+      <c r="AE17" s="3">
+        <f>9+2</f>
+        <v>11</v>
+      </c>
+      <c r="AF17" s="3">
         <v>0</v>
       </c>
-      <c r="AB17" s="3">
+      <c r="AG17" s="3">
         <v>0</v>
       </c>
-      <c r="AC17" s="3">
+      <c r="AH17" s="3">
         <v>513</v>
       </c>
-      <c r="AD17" s="3">
+      <c r="AI17" s="3">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="AJ17" s="3">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="18" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>34</v>
       </c>
-      <c r="J18" s="10">
-        <f>J16-J17</f>
+      <c r="J18" s="10"/>
+      <c r="K18" s="10">
+        <f>K16-K17</f>
         <v>1179</v>
       </c>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
+      <c r="L18" s="10">
+        <f>L16-L17</f>
+        <v>1460</v>
+      </c>
+      <c r="M18" s="10">
+        <f>M16-M17</f>
+        <v>935</v>
+      </c>
+      <c r="N18" s="10">
+        <f t="shared" ref="N18" si="13">N16-N17</f>
+        <v>890</v>
+      </c>
       <c r="O18" s="10">
-        <f>O16-O17</f>
+        <f t="shared" ref="O18:T18" si="14">O16-O17</f>
         <v>673</v>
       </c>
-      <c r="AA18" s="3">
-        <f>+AA16-AA17</f>
+      <c r="P18" s="10">
+        <f t="shared" si="14"/>
+        <v>706</v>
+      </c>
+      <c r="Q18" s="10">
+        <f t="shared" si="14"/>
+        <v>946</v>
+      </c>
+      <c r="R18" s="10">
+        <f t="shared" si="14"/>
+        <v>598</v>
+      </c>
+      <c r="S18" s="10">
+        <f t="shared" si="14"/>
+        <v>621</v>
+      </c>
+      <c r="T18" s="10">
+        <f t="shared" si="14"/>
+        <v>851</v>
+      </c>
+      <c r="AD18" s="3">
+        <f t="shared" ref="AD18:AJ18" si="15">+AD16-AD17</f>
+        <v>19</v>
+      </c>
+      <c r="AE18" s="3">
+        <f t="shared" si="15"/>
+        <v>319</v>
+      </c>
+      <c r="AF18" s="3">
+        <f t="shared" si="15"/>
         <v>312</v>
       </c>
-      <c r="AB18" s="3">
-        <f>+AB16-AB17</f>
+      <c r="AG18" s="3">
+        <f t="shared" si="15"/>
         <v>1275</v>
       </c>
-      <c r="AC18" s="3">
-        <f>+AC16-AC17</f>
+      <c r="AH18" s="3">
+        <f t="shared" si="15"/>
         <v>3144</v>
       </c>
-      <c r="AD18" s="3">
-        <f>+AD16-AD17</f>
+      <c r="AI18" s="3">
+        <f t="shared" si="15"/>
         <v>4630</v>
       </c>
-    </row>
-    <row r="19" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="AJ18" s="3">
+        <f t="shared" si="15"/>
+        <v>2923</v>
+      </c>
+    </row>
+    <row r="19" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>24</v>
       </c>
-      <c r="J19" s="11">
-        <f>J18/J20</f>
+      <c r="J19" s="11"/>
+      <c r="K19" s="11">
+        <f t="shared" ref="K19:T19" si="16">K18/K20</f>
         <v>0.83617021276595749</v>
       </c>
+      <c r="L19" s="11">
+        <f t="shared" si="16"/>
+        <v>0.89460784313725494</v>
+      </c>
+      <c r="M19" s="11">
+        <f t="shared" si="16"/>
+        <v>0.58038485412787089</v>
+      </c>
+      <c r="N19" s="11">
+        <f t="shared" si="16"/>
+        <v>0.56651814131126665</v>
+      </c>
       <c r="O19" s="11">
-        <f>O18/O20</f>
+        <f t="shared" si="16"/>
         <v>0.41775294847920547</v>
       </c>
-      <c r="AA19" s="1">
-        <f>+AA18/AA20</f>
+      <c r="P19" s="11">
+        <f t="shared" si="16"/>
+        <v>0.4339274738783036</v>
+      </c>
+      <c r="Q19" s="11">
+        <f t="shared" si="16"/>
+        <v>0.58072437077961936</v>
+      </c>
+      <c r="R19" s="11">
+        <f t="shared" si="16"/>
+        <v>0.36799999999999999</v>
+      </c>
+      <c r="S19" s="11">
+        <f t="shared" si="16"/>
+        <v>0.37888956680902991</v>
+      </c>
+      <c r="T19" s="11">
+        <f t="shared" si="16"/>
+        <v>0.51985339034819789</v>
+      </c>
+      <c r="AD19" s="1">
+        <f t="shared" ref="AD19:AJ19" si="17">+AD18/AD20</f>
+        <v>1.9957983193277309E-2</v>
+      </c>
+      <c r="AE19" s="1">
+        <f t="shared" si="17"/>
+        <v>0.29981203007518797</v>
+      </c>
+      <c r="AF19" s="1">
+        <f t="shared" si="17"/>
         <v>0.27857142857142858</v>
       </c>
-      <c r="AB19" s="1">
-        <f>+AB18/AB20</f>
+      <c r="AG19" s="1">
+        <f t="shared" si="17"/>
         <v>1.056338028169014</v>
       </c>
-      <c r="AC19" s="1">
-        <f>+AC18/AC20</f>
+      <c r="AH19" s="1">
+        <f t="shared" si="17"/>
         <v>2.5581773799837264</v>
       </c>
-      <c r="AD19" s="1">
-        <f>+AD18/AD20</f>
+      <c r="AI19" s="1">
+        <f t="shared" si="17"/>
         <v>2.9471674092934435</v>
       </c>
-    </row>
-    <row r="20" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="AJ19" s="1">
+        <f t="shared" si="17"/>
+        <v>1.7987692307692307</v>
+      </c>
+    </row>
+    <row r="20" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>1</v>
       </c>
-      <c r="J20" s="10">
+      <c r="J20" s="10"/>
+      <c r="K20" s="10">
         <v>1410</v>
       </c>
-      <c r="K20" s="10"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
-      <c r="N20" s="10"/>
+      <c r="L20" s="10">
+        <v>1632</v>
+      </c>
+      <c r="M20" s="10">
+        <v>1611</v>
+      </c>
+      <c r="N20" s="10">
+        <f>+AI20</f>
+        <v>1571</v>
+      </c>
       <c r="O20" s="10">
         <v>1611</v>
       </c>
-      <c r="AA20" s="3">
+      <c r="P20" s="10">
+        <v>1627</v>
+      </c>
+      <c r="Q20" s="10">
+        <v>1629</v>
+      </c>
+      <c r="R20" s="10">
+        <f>+AJ20</f>
+        <v>1625</v>
+      </c>
+      <c r="S20" s="10">
+        <v>1639</v>
+      </c>
+      <c r="T20" s="10">
+        <v>1637</v>
+      </c>
+      <c r="AD20" s="3">
+        <v>952</v>
+      </c>
+      <c r="AE20" s="3">
+        <v>1064</v>
+      </c>
+      <c r="AF20" s="3">
         <v>1120</v>
       </c>
-      <c r="AB20" s="3">
+      <c r="AG20" s="3">
         <v>1207</v>
       </c>
-      <c r="AC20" s="3">
+      <c r="AH20" s="3">
         <v>1229</v>
       </c>
-      <c r="AD20" s="3">
+      <c r="AI20" s="3">
         <v>1571</v>
       </c>
-    </row>
-    <row r="23" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="AJ20" s="3">
+        <v>1625</v>
+      </c>
+    </row>
+    <row r="23" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>35</v>
       </c>
+      <c r="N23" s="12"/>
       <c r="O23" s="12">
-        <f>O8/J8-1</f>
+        <f>O8/K8-1</f>
         <v>-9.0708340411075228E-2</v>
       </c>
+      <c r="P23" s="12">
+        <f t="shared" ref="P23:T23" si="18">P8/L8-1</f>
+        <v>-0.18183206106870231</v>
+      </c>
+      <c r="Q23" s="12">
+        <f t="shared" si="18"/>
+        <v>4.2228212039532753E-2</v>
+      </c>
+      <c r="R23" s="12">
+        <f t="shared" si="18"/>
+        <v>0.10162529023039824</v>
+      </c>
+      <c r="S23" s="12">
+        <f t="shared" si="18"/>
+        <v>2.2417336073230043E-2</v>
+      </c>
+      <c r="T23" s="12">
+        <f t="shared" si="18"/>
+        <v>8.882254151894009E-2</v>
+      </c>
+      <c r="AA23" s="7">
+        <f t="shared" ref="AA23:AD23" si="19">+AA8/Z8-1</f>
+        <v>3.9063974334780038E-2</v>
+      </c>
       <c r="AB23" s="7">
-        <f>+AB8/AA8-1</f>
+        <f t="shared" si="19"/>
+        <v>-0.27515437704322554</v>
+      </c>
+      <c r="AC23" s="7">
+        <f t="shared" si="19"/>
+        <v>7.0408418942620843E-2</v>
+      </c>
+      <c r="AD23" s="7">
+        <f t="shared" si="19"/>
+        <v>0.24742509363295873</v>
+      </c>
+      <c r="AE23" s="7">
+        <f t="shared" ref="AE23:AJ23" si="20">+AE8/AD8-1</f>
+        <v>0.21504972790392185</v>
+      </c>
+      <c r="AF23" s="7">
+        <f t="shared" si="20"/>
+        <v>3.9536679536679609E-2</v>
+      </c>
+      <c r="AG23" s="7">
+        <f t="shared" si="20"/>
         <v>0.45045312732134901</v>
       </c>
-      <c r="AC23" s="7">
-        <f>+AC8/AB8-1</f>
+      <c r="AH23" s="7">
+        <f t="shared" si="20"/>
         <v>0.68329406944586712</v>
       </c>
-      <c r="AD23" s="7">
-        <f>+AD8/AC8-1</f>
+      <c r="AI23" s="7">
+        <f t="shared" si="20"/>
         <v>0.43610806863818907</v>
       </c>
-    </row>
-    <row r="25" spans="2:30" x14ac:dyDescent="0.2">
+      <c r="AJ23" s="7">
+        <f t="shared" si="20"/>
+        <v>-3.9023770179229644E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:36" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>26</v>
       </c>
-      <c r="J25" s="12">
-        <f>J10/J8</f>
+      <c r="J25" s="12"/>
+      <c r="K25" s="12">
+        <f>K10/K8</f>
         <v>0.51027688126380155</v>
+      </c>
+      <c r="L25" s="12">
+        <f>L10/L8</f>
+        <v>0.52442748091603053</v>
+      </c>
+      <c r="M25" s="12">
+        <f t="shared" ref="M25:N25" si="21">M10/M8</f>
+        <v>0.49703504043126684</v>
+      </c>
+      <c r="N25" s="12">
+        <f t="shared" si="21"/>
+        <v>0.5083050544740132</v>
       </c>
       <c r="O25" s="12">
         <f>O10/O8</f>
         <v>0.49766486082570521</v>
+      </c>
+      <c r="P25" s="12">
+        <f t="shared" ref="P25:T25" si="22">P10/P8</f>
+        <v>0.49542825153946629</v>
+      </c>
+      <c r="Q25" s="12">
+        <f t="shared" si="22"/>
+        <v>0.5098275862068965</v>
+      </c>
+      <c r="R25" s="12">
+        <f t="shared" si="22"/>
+        <v>0.50680933852140075</v>
+      </c>
+      <c r="S25" s="12">
+        <f t="shared" si="22"/>
+        <v>0.5097752603690846</v>
+      </c>
+      <c r="T25" s="12">
+        <f t="shared" si="22"/>
+        <v>0.53041988003427587</v>
+      </c>
+      <c r="AD25" s="7">
+        <f>+AD10/AD8</f>
+        <v>0.3495965471945956</v>
+      </c>
+      <c r="AE25" s="7">
+        <f>+AE10/AE8</f>
+        <v>0.37791505791505792</v>
+      </c>
+      <c r="AF25" s="7">
+        <f>+AF10/AF8</f>
+        <v>0.42608824840291187</v>
+      </c>
+      <c r="AG25" s="7">
+        <f t="shared" ref="AG25:AJ25" si="23">+AG10/AG8</f>
+        <v>0.44525248386766364</v>
+      </c>
+      <c r="AH25" s="7">
+        <f t="shared" si="23"/>
+        <v>0.48247535596933189</v>
+      </c>
+      <c r="AI25" s="7">
+        <f t="shared" si="23"/>
+        <v>0.51061395703571888</v>
+      </c>
+      <c r="AJ25" s="7">
+        <f t="shared" si="23"/>
+        <v>0.5027336860670194</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PG and other updates
</commit_message>
<xml_diff>
--- a/AMD.xlsx
+++ b/AMD.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shkre\code\models\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Martin Shkreli - DL\models\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8921E28-F623-45F8-AFB9-E5F319E9EF15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6D4EB25-3164-4A44-B08B-C8CC0F792A80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26820" yWindow="780" windowWidth="26220" windowHeight="14910" activeTab="1" xr2:uid="{449F5976-BBB2-4D6E-9B28-E8B6EC62A528}"/>
+    <workbookView xWindow="17955" yWindow="1035" windowWidth="19965" windowHeight="11010" activeTab="1" xr2:uid="{449F5976-BBB2-4D6E-9B28-E8B6EC62A528}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="94">
   <si>
     <t>Price</t>
   </si>
@@ -199,6 +199,126 @@
   </si>
   <si>
     <t>ONCA</t>
+  </si>
+  <si>
+    <t>Q125</t>
+  </si>
+  <si>
+    <t>Q225</t>
+  </si>
+  <si>
+    <t>Q325</t>
+  </si>
+  <si>
+    <t>Q425</t>
+  </si>
+  <si>
+    <t>L+SE</t>
+  </si>
+  <si>
+    <t>SE</t>
+  </si>
+  <si>
+    <t>OLTL</t>
+  </si>
+  <si>
+    <t>DT</t>
+  </si>
+  <si>
+    <t>Leases</t>
+  </si>
+  <si>
+    <t>OCL</t>
+  </si>
+  <si>
+    <t>AL</t>
+  </si>
+  <si>
+    <t>Related</t>
+  </si>
+  <si>
+    <t>AP</t>
+  </si>
+  <si>
+    <t>Net Debt</t>
+  </si>
+  <si>
+    <t>Instinct GPU</t>
+  </si>
+  <si>
+    <t>EPYC CPU</t>
+  </si>
+  <si>
+    <t>Ryzen CPU</t>
+  </si>
+  <si>
+    <t>Radeon GPU</t>
+  </si>
+  <si>
+    <t>MI300X</t>
+  </si>
+  <si>
+    <t>MI300</t>
+  </si>
+  <si>
+    <t>ROCm</t>
+  </si>
+  <si>
+    <t>LiquidAI, Vultr, Absci</t>
+  </si>
+  <si>
+    <t>Ryzen AI PRO</t>
+  </si>
+  <si>
+    <t>Dell Pro notebook/desktop PC partnership</t>
+  </si>
+  <si>
+    <t>Ryzen AI Max, Max PRO</t>
+  </si>
+  <si>
+    <t>Ryzen AI 300</t>
+  </si>
+  <si>
+    <t>Ryzen AI 300 PRO</t>
+  </si>
+  <si>
+    <t>notebook</t>
+  </si>
+  <si>
+    <t>Ryzen 200</t>
+  </si>
+  <si>
+    <t>Ryzen 200 PRO</t>
+  </si>
+  <si>
+    <t>MI300A</t>
+  </si>
+  <si>
+    <t>Ryzen 9000HX - handheld</t>
+  </si>
+  <si>
+    <t>Ryzen Z2 - mobile</t>
+  </si>
+  <si>
+    <t>Ryzen 9000X3D - desktop</t>
+  </si>
+  <si>
+    <t>Versal FPGA</t>
+  </si>
+  <si>
+    <t>CXL 3.1, PCIe Gen6, LPDDR5X</t>
+  </si>
+  <si>
+    <t>Versal RF</t>
+  </si>
+  <si>
+    <t>CFFO</t>
+  </si>
+  <si>
+    <t>CX</t>
+  </si>
+  <si>
+    <t>FCF</t>
   </si>
 </sst>
 </file>
@@ -248,7 +368,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -274,6 +394,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -298,16 +419,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>48986</xdr:colOff>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>42416</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>48986</xdr:colOff>
-      <xdr:row>40</xdr:row>
-      <xdr:rowOff>10886</xdr:rowOff>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>42416</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>59121</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -322,8 +443,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="22315715" y="0"/>
-          <a:ext cx="0" cy="6542315"/>
+          <a:off x="26022675" y="0"/>
+          <a:ext cx="0" cy="10569466"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -348,16 +469,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>46618</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>59755</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>21771</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>46618</xdr:colOff>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>59755</xdr:colOff>
       <xdr:row>71</xdr:row>
-      <xdr:rowOff>132522</xdr:rowOff>
+      <xdr:rowOff>110751</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -372,8 +493,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="13232531" y="21771"/>
-          <a:ext cx="0" cy="11872055"/>
+          <a:off x="13821738" y="0"/>
+          <a:ext cx="0" cy="11770665"/>
         </a:xfrm>
         <a:prstGeom prst="line">
           <a:avLst/>
@@ -696,72 +817,169 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C60D5A4-2898-4A25-B128-984AAEABB5C4}">
-  <dimension ref="L2:N7"/>
+  <dimension ref="B2:N24"/>
   <sheetViews>
-    <sheetView zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="2" spans="12:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="F2" t="s">
+        <v>88</v>
+      </c>
       <c r="L2" t="s">
         <v>0</v>
       </c>
       <c r="M2" s="1">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="3" spans="12:14" x14ac:dyDescent="0.2">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>68</v>
+      </c>
+      <c r="F3" t="s">
+        <v>89</v>
+      </c>
       <c r="L3" t="s">
         <v>1</v>
       </c>
       <c r="M3" s="3">
-        <v>1618</v>
+        <v>1634</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="12:14" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" t="s">
+        <v>90</v>
+      </c>
       <c r="L4" t="s">
         <v>2</v>
       </c>
       <c r="M4" s="3">
         <f>+M2*M3</f>
-        <v>131058</v>
-      </c>
-    </row>
-    <row r="5" spans="12:14" x14ac:dyDescent="0.2">
+        <v>156864</v>
+      </c>
+    </row>
+    <row r="5" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C5" t="s">
+        <v>73</v>
+      </c>
       <c r="L5" t="s">
         <v>3</v>
       </c>
       <c r="M5" s="3">
-        <f>4835+1020</f>
-        <v>5855</v>
+        <v>5281</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="12:14" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C6" t="s">
+        <v>74</v>
+      </c>
       <c r="L6" t="s">
         <v>4</v>
       </c>
       <c r="M6" s="3">
-        <v>2467</v>
+        <v>1721</v>
       </c>
       <c r="N6" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="7" spans="12:14" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C7" t="s">
+        <v>84</v>
+      </c>
       <c r="L7" t="s">
         <v>5</v>
       </c>
       <c r="M7" s="3">
         <f>+M4-M5+M6</f>
-        <v>127670</v>
+        <v>153304</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>70</v>
+      </c>
+      <c r="M8" s="3"/>
+    </row>
+    <row r="9" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C11" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="12" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C13" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="14" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="15" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B19" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B20" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="24" spans="2:3" x14ac:dyDescent="0.2">
+      <c r="B24" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -771,28 +989,28 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00C865FD-8E44-4C73-A775-FD93E4059E5E}">
-  <dimension ref="A1:AS51"/>
+  <dimension ref="A1:AX54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="N37" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="2" topLeftCell="AK3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="U45" sqref="U45"/>
+      <selection pane="bottomRight" activeCell="AR5" sqref="AR5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="23" width="9.140625" style="2"/>
+    <col min="3" max="28" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A1" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
       <c r="C2" s="2" t="s">
         <v>8</v>
       </c>
@@ -853,85 +1071,97 @@
       <c r="V2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Z2">
+      <c r="W2" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="X2" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE2">
         <v>2013</v>
       </c>
-      <c r="AA2">
+      <c r="AF2">
         <v>2014</v>
       </c>
-      <c r="AB2">
+      <c r="AG2">
         <v>2015</v>
       </c>
-      <c r="AC2">
-        <f>+AB2+1</f>
+      <c r="AH2">
+        <f>+AG2+1</f>
         <v>2016</v>
       </c>
-      <c r="AD2">
-        <f t="shared" ref="AD2:AS2" si="0">+AC2+1</f>
+      <c r="AI2">
+        <f t="shared" ref="AI2:AX2" si="0">+AH2+1</f>
         <v>2017</v>
       </c>
-      <c r="AE2">
+      <c r="AJ2">
         <f t="shared" si="0"/>
         <v>2018</v>
       </c>
-      <c r="AF2">
+      <c r="AK2">
         <f t="shared" si="0"/>
         <v>2019</v>
       </c>
-      <c r="AG2">
+      <c r="AL2">
         <f t="shared" si="0"/>
         <v>2020</v>
       </c>
-      <c r="AH2">
+      <c r="AM2">
         <f t="shared" si="0"/>
         <v>2021</v>
       </c>
-      <c r="AI2">
+      <c r="AN2">
         <f t="shared" si="0"/>
         <v>2022</v>
       </c>
-      <c r="AJ2">
+      <c r="AO2">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="AK2">
+      <c r="AP2">
         <f t="shared" si="0"/>
         <v>2024</v>
       </c>
-      <c r="AL2">
+      <c r="AQ2">
         <f t="shared" si="0"/>
         <v>2025</v>
       </c>
-      <c r="AM2">
+      <c r="AR2">
         <f t="shared" si="0"/>
         <v>2026</v>
       </c>
-      <c r="AN2">
+      <c r="AS2">
         <f t="shared" si="0"/>
         <v>2027</v>
       </c>
-      <c r="AO2">
+      <c r="AT2">
         <f t="shared" si="0"/>
         <v>2028</v>
       </c>
-      <c r="AP2">
+      <c r="AU2">
         <f t="shared" si="0"/>
         <v>2029</v>
       </c>
-      <c r="AQ2">
+      <c r="AV2">
         <f t="shared" si="0"/>
         <v>2030</v>
       </c>
-      <c r="AR2">
+      <c r="AW2">
         <f t="shared" si="0"/>
         <v>2031</v>
       </c>
-      <c r="AS2">
+      <c r="AX2">
         <f t="shared" si="0"/>
         <v>2032</v>
       </c>
     </row>
-    <row r="3" spans="1:45" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>36</v>
       </c>
@@ -954,14 +1184,21 @@
       <c r="T3" s="10">
         <v>2834</v>
       </c>
-      <c r="AI3" s="3">
+      <c r="U3" s="10"/>
+      <c r="V3" s="10">
+        <v>3900</v>
+      </c>
+      <c r="AN3" s="3">
         <v>6043</v>
       </c>
-      <c r="AJ3" s="3">
+      <c r="AO3" s="3">
         <v>6496</v>
       </c>
-    </row>
-    <row r="4" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AP3" s="3">
+        <v>12600</v>
+      </c>
+    </row>
+    <row r="4" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
         <v>37</v>
       </c>
@@ -981,14 +1218,21 @@
       <c r="T4" s="10">
         <v>1492</v>
       </c>
-      <c r="AI4" s="3">
+      <c r="U4" s="10"/>
+      <c r="V4" s="10">
+        <v>2300</v>
+      </c>
+      <c r="AN4" s="3">
         <v>6201</v>
       </c>
-      <c r="AJ4" s="3">
+      <c r="AO4" s="3">
         <v>4651</v>
       </c>
-    </row>
-    <row r="5" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AP4" s="3">
+        <v>7100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
         <v>38</v>
       </c>
@@ -1011,14 +1255,20 @@
       <c r="T5" s="10">
         <v>648</v>
       </c>
-      <c r="AI5" s="3">
+      <c r="V5" s="2">
+        <v>563</v>
+      </c>
+      <c r="AN5" s="3">
         <v>6805</v>
       </c>
-      <c r="AJ5" s="3">
+      <c r="AO5" s="3">
         <v>6212</v>
       </c>
-    </row>
-    <row r="6" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AP5" s="3">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="6" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>39</v>
       </c>
@@ -1041,18 +1291,24 @@
       <c r="T6" s="10">
         <v>861</v>
       </c>
-      <c r="AI6" s="3">
+      <c r="V6" s="2">
+        <v>923</v>
+      </c>
+      <c r="AN6" s="3">
         <v>4552</v>
       </c>
-      <c r="AJ6" s="3">
+      <c r="AO6" s="3">
         <v>5321</v>
       </c>
-    </row>
-    <row r="7" spans="1:45" x14ac:dyDescent="0.2">
-      <c r="AI7" s="3"/>
-      <c r="AJ7" s="3"/>
-    </row>
-    <row r="8" spans="1:45" s="4" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="AP6" s="3">
+        <v>3600</v>
+      </c>
+    </row>
+    <row r="7" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="AN7" s="3"/>
+      <c r="AO7" s="3"/>
+    </row>
+    <row r="8" spans="1:50" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
@@ -1074,7 +1330,7 @@
         <v>5565</v>
       </c>
       <c r="N8" s="9">
-        <f>+AI8-M8-L8-K8</f>
+        <f>+AN8-M8-L8-K8</f>
         <v>5599</v>
       </c>
       <c r="O8" s="9">
@@ -1087,7 +1343,7 @@
         <v>5800</v>
       </c>
       <c r="R8" s="9">
-        <f>+AJ8-Q8-P8-O8</f>
+        <f>+AO8-Q8-P8-O8</f>
         <v>6168</v>
       </c>
       <c r="S8" s="9">
@@ -1099,44 +1355,57 @@
       <c r="U8" s="9">
         <v>6819</v>
       </c>
-      <c r="V8" s="5"/>
-      <c r="W8" s="5"/>
-      <c r="Z8" s="6">
+      <c r="V8" s="9">
+        <v>7658</v>
+      </c>
+      <c r="W8" s="9">
+        <v>7100</v>
+      </c>
+      <c r="X8" s="5"/>
+      <c r="Y8" s="5"/>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="5"/>
+      <c r="AB8" s="5"/>
+      <c r="AE8" s="6">
         <v>5299</v>
       </c>
-      <c r="AA8" s="6">
+      <c r="AF8" s="6">
         <v>5506</v>
       </c>
-      <c r="AB8" s="6">
+      <c r="AG8" s="6">
         <v>3991</v>
       </c>
-      <c r="AC8" s="6">
+      <c r="AH8" s="6">
         <v>4272</v>
       </c>
-      <c r="AD8" s="6">
+      <c r="AI8" s="6">
         <v>5329</v>
       </c>
-      <c r="AE8" s="6">
+      <c r="AJ8" s="6">
         <v>6475</v>
       </c>
-      <c r="AF8" s="6">
+      <c r="AK8" s="6">
         <v>6731</v>
       </c>
-      <c r="AG8" s="6">
+      <c r="AL8" s="6">
         <v>9763</v>
       </c>
-      <c r="AH8" s="6">
+      <c r="AM8" s="6">
         <v>16434</v>
       </c>
-      <c r="AI8" s="6">
+      <c r="AN8" s="6">
         <v>23601</v>
       </c>
-      <c r="AJ8" s="6">
-        <f>SUM(AJ3:AJ6)</f>
+      <c r="AO8" s="6">
+        <f>SUM(AO3:AO6)</f>
         <v>22680</v>
       </c>
-    </row>
-    <row r="9" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AP8" s="6">
+        <f>SUM(S8:V8)</f>
+        <v>25785</v>
+      </c>
+    </row>
+    <row r="9" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B9" t="s">
         <v>25</v>
       </c>
@@ -1151,7 +1420,7 @@
         <v>2799</v>
       </c>
       <c r="N9" s="10">
-        <f>+AI9-M9-L9-K9</f>
+        <f>+AN9-M9-L9-K9</f>
         <v>2753</v>
       </c>
       <c r="O9" s="10">
@@ -1164,7 +1433,7 @@
         <v>2843</v>
       </c>
       <c r="R9" s="10">
-        <f>+AJ9-Q9-P9-O9</f>
+        <f>+AO9-Q9-P9-O9</f>
         <v>3042</v>
       </c>
       <c r="S9" s="10">
@@ -1176,29 +1445,36 @@
       <c r="U9" s="10">
         <v>3167</v>
       </c>
-      <c r="AD9" s="3">
+      <c r="V9" s="10">
+        <v>3524</v>
+      </c>
+      <c r="AI9" s="3">
         <v>3466</v>
       </c>
-      <c r="AE9" s="3">
+      <c r="AJ9" s="3">
         <v>4028</v>
       </c>
-      <c r="AF9" s="3">
+      <c r="AK9" s="3">
         <v>3863</v>
       </c>
-      <c r="AG9" s="3">
+      <c r="AL9" s="3">
         <v>5416</v>
       </c>
-      <c r="AH9" s="3">
+      <c r="AM9" s="3">
         <v>8505</v>
       </c>
-      <c r="AI9" s="3">
+      <c r="AN9" s="3">
         <v>11550</v>
       </c>
-      <c r="AJ9" s="3">
+      <c r="AO9" s="3">
         <v>11278</v>
       </c>
-    </row>
-    <row r="10" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AP9" s="13">
+        <f>SUM(S9:V9)</f>
+        <v>12114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B10" t="s">
         <v>26</v>
       </c>
@@ -1247,36 +1523,44 @@
         <f>+U8-U9</f>
         <v>3652</v>
       </c>
-      <c r="AD10" s="3">
-        <f t="shared" ref="AD10:AJ10" si="2">+AD8-AD9</f>
+      <c r="V10" s="10">
+        <f>+V8-V9</f>
+        <v>4134</v>
+      </c>
+      <c r="AI10" s="3">
+        <f t="shared" ref="AI10:AO10" si="2">+AI8-AI9</f>
         <v>1863</v>
       </c>
-      <c r="AE10" s="3">
+      <c r="AJ10" s="3">
         <f t="shared" si="2"/>
         <v>2447</v>
       </c>
-      <c r="AF10" s="3">
+      <c r="AK10" s="3">
         <f t="shared" si="2"/>
         <v>2868</v>
       </c>
-      <c r="AG10" s="3">
+      <c r="AL10" s="3">
         <f t="shared" si="2"/>
         <v>4347</v>
       </c>
-      <c r="AH10" s="3">
+      <c r="AM10" s="3">
         <f t="shared" si="2"/>
         <v>7929</v>
       </c>
-      <c r="AI10" s="3">
+      <c r="AN10" s="3">
         <f t="shared" si="2"/>
         <v>12051</v>
       </c>
-      <c r="AJ10" s="3">
+      <c r="AO10" s="3">
         <f t="shared" si="2"/>
         <v>11402</v>
       </c>
-    </row>
-    <row r="11" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AP10" s="3">
+        <f>+AP8-AP9</f>
+        <v>13671</v>
+      </c>
+    </row>
+    <row r="11" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>27</v>
       </c>
@@ -1291,7 +1575,7 @@
         <v>1279</v>
       </c>
       <c r="N11" s="10">
-        <f t="shared" ref="N11:N12" si="3">+AI11-M11-L11-K11</f>
+        <f t="shared" ref="N11:N12" si="3">+AN11-M11-L11-K11</f>
         <v>1366</v>
       </c>
       <c r="O11" s="10">
@@ -1304,7 +1588,7 @@
         <v>1507</v>
       </c>
       <c r="R11" s="10">
-        <f>+AJ11-Q11-P11-O11</f>
+        <f>+AO11-Q11-P11-O11</f>
         <v>1511</v>
       </c>
       <c r="S11" s="10">
@@ -1316,29 +1600,36 @@
       <c r="U11" s="10">
         <v>1636</v>
       </c>
-      <c r="AD11" s="3">
+      <c r="V11" s="10">
+        <v>1712</v>
+      </c>
+      <c r="AI11" s="3">
         <v>1196</v>
       </c>
-      <c r="AE11" s="3">
+      <c r="AJ11" s="3">
         <v>1434</v>
       </c>
-      <c r="AF11" s="3">
+      <c r="AK11" s="3">
         <v>1547</v>
       </c>
-      <c r="AG11" s="3">
+      <c r="AL11" s="3">
         <v>1983</v>
       </c>
-      <c r="AH11" s="3">
+      <c r="AM11" s="3">
         <v>2845</v>
       </c>
-      <c r="AI11" s="3">
+      <c r="AN11" s="3">
         <v>5005</v>
       </c>
-      <c r="AJ11" s="3">
+      <c r="AO11" s="3">
         <v>5872</v>
       </c>
-    </row>
-    <row r="12" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AP11" s="13">
+        <f t="shared" ref="AP11:AP12" si="4">SUM(S11:V11)</f>
+        <v>6456</v>
+      </c>
+    </row>
+    <row r="12" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B12" t="s">
         <v>28</v>
       </c>
@@ -1366,7 +1657,7 @@
         <v>576</v>
       </c>
       <c r="R12" s="10">
-        <f>+AJ12-Q12-P12-O12</f>
+        <f>+AO12-Q12-P12-O12</f>
         <v>644</v>
       </c>
       <c r="S12" s="10">
@@ -1378,29 +1669,36 @@
       <c r="U12" s="10">
         <v>721</v>
       </c>
-      <c r="AD12" s="3">
+      <c r="V12" s="10">
+        <v>792</v>
+      </c>
+      <c r="AI12" s="3">
         <v>516</v>
       </c>
-      <c r="AE12" s="3">
+      <c r="AJ12" s="3">
         <v>562</v>
       </c>
-      <c r="AF12" s="3">
+      <c r="AK12" s="3">
         <v>750</v>
       </c>
-      <c r="AG12" s="3">
+      <c r="AL12" s="3">
         <v>995</v>
       </c>
-      <c r="AH12" s="3">
+      <c r="AM12" s="3">
         <v>1448</v>
       </c>
-      <c r="AI12" s="3">
+      <c r="AN12" s="3">
         <v>2336</v>
       </c>
-      <c r="AJ12" s="3">
+      <c r="AO12" s="3">
         <v>2352</v>
       </c>
-    </row>
-    <row r="13" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AP12" s="13">
+        <f t="shared" si="4"/>
+        <v>2783</v>
+      </c>
+    </row>
+    <row r="13" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
         <v>29</v>
       </c>
@@ -1418,67 +1716,75 @@
         <v>1836</v>
       </c>
       <c r="N13" s="10">
-        <f t="shared" ref="N13" si="4">N11+N12</f>
+        <f t="shared" ref="N13" si="5">N11+N12</f>
         <v>1956</v>
       </c>
       <c r="O13" s="10">
-        <f t="shared" ref="O13:U13" si="5">O11+O12</f>
+        <f t="shared" ref="O13:U13" si="6">O11+O12</f>
         <v>1996</v>
       </c>
       <c r="P13" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1990</v>
       </c>
       <c r="Q13" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2083</v>
       </c>
       <c r="R13" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2155</v>
       </c>
       <c r="S13" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2145</v>
       </c>
       <c r="T13" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2233</v>
       </c>
       <c r="U13" s="10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2357</v>
       </c>
-      <c r="AD13" s="3">
-        <f>+AD11+AD12</f>
+      <c r="V13" s="10">
+        <f t="shared" ref="V13" si="7">V11+V12</f>
+        <v>2504</v>
+      </c>
+      <c r="AI13" s="3">
+        <f>+AI11+AI12</f>
         <v>1712</v>
       </c>
-      <c r="AE13" s="3">
-        <f>+AE11+AE12</f>
+      <c r="AJ13" s="3">
+        <f>+AJ11+AJ12</f>
         <v>1996</v>
       </c>
-      <c r="AF13" s="3">
-        <f>+AF11+AF12</f>
+      <c r="AK13" s="3">
+        <f>+AK11+AK12</f>
         <v>2297</v>
       </c>
-      <c r="AG13" s="3">
-        <f>+AG11+AG12</f>
+      <c r="AL13" s="3">
+        <f>+AL11+AL12</f>
         <v>2978</v>
       </c>
-      <c r="AH13" s="3">
-        <f>+AH11+AH12</f>
+      <c r="AM13" s="3">
+        <f>+AM11+AM12</f>
         <v>4293</v>
       </c>
-      <c r="AI13" s="3">
-        <f t="shared" ref="AI13:AJ13" si="6">+AI11+AI12</f>
+      <c r="AN13" s="3">
+        <f t="shared" ref="AN13:AO13" si="8">+AN11+AN12</f>
         <v>7341</v>
       </c>
-      <c r="AJ13" s="3">
-        <f t="shared" si="6"/>
+      <c r="AO13" s="3">
+        <f t="shared" si="8"/>
         <v>8224</v>
       </c>
-    </row>
-    <row r="14" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AP13" s="3">
+        <f t="shared" ref="AP13" si="9">+AP11+AP12</f>
+        <v>9239</v>
+      </c>
+    </row>
+    <row r="14" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B14" t="s">
         <v>30</v>
       </c>
@@ -1496,67 +1802,75 @@
         <v>930</v>
       </c>
       <c r="N14" s="10">
-        <f t="shared" ref="N14" si="7">N10-N13</f>
+        <f t="shared" ref="N14" si="10">N10-N13</f>
         <v>890</v>
       </c>
       <c r="O14" s="10">
-        <f t="shared" ref="O14:U14" si="8">O10-O13</f>
+        <f t="shared" ref="O14:U14" si="11">O10-O13</f>
         <v>668</v>
       </c>
       <c r="P14" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>665</v>
       </c>
       <c r="Q14" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>874</v>
       </c>
       <c r="R14" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>971</v>
       </c>
       <c r="S14" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>645</v>
       </c>
       <c r="T14" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>862</v>
       </c>
       <c r="U14" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>1295</v>
       </c>
-      <c r="AD14" s="3">
-        <f>+AD10-AD13</f>
+      <c r="V14" s="10">
+        <f t="shared" ref="V14" si="12">V10-V13</f>
+        <v>1630</v>
+      </c>
+      <c r="AI14" s="3">
+        <f>+AI10-AI13</f>
         <v>151</v>
       </c>
-      <c r="AE14" s="3">
-        <f>+AE10-AE13</f>
+      <c r="AJ14" s="3">
+        <f>+AJ10-AJ13</f>
         <v>451</v>
       </c>
-      <c r="AF14" s="3">
-        <f>+AF10-AF13</f>
+      <c r="AK14" s="3">
+        <f>+AK10-AK13</f>
         <v>571</v>
       </c>
-      <c r="AG14" s="3">
-        <f>+AG10-AG13</f>
+      <c r="AL14" s="3">
+        <f>+AL10-AL13</f>
         <v>1369</v>
       </c>
-      <c r="AH14" s="3">
-        <f>+AH10-AH13</f>
+      <c r="AM14" s="3">
+        <f>+AM10-AM13</f>
         <v>3636</v>
       </c>
-      <c r="AI14" s="3">
-        <f t="shared" ref="AI14:AJ14" si="9">+AI10-AI13</f>
+      <c r="AN14" s="3">
+        <f t="shared" ref="AN14:AO14" si="13">+AN10-AN13</f>
         <v>4710</v>
       </c>
-      <c r="AJ14" s="3">
-        <f t="shared" si="9"/>
+      <c r="AO14" s="3">
+        <f t="shared" si="13"/>
         <v>3178</v>
       </c>
-    </row>
-    <row r="15" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AP14" s="3">
+        <f t="shared" ref="AP14" si="14">+AP10-AP13</f>
+        <v>4432</v>
+      </c>
+    </row>
+    <row r="15" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B15" t="s">
         <v>31</v>
       </c>
@@ -1587,7 +1901,7 @@
         <v>33</v>
       </c>
       <c r="R15" s="10">
-        <f>+AJ15-Q15-P15-O15</f>
+        <f>+AO15-Q15-P15-O15</f>
         <v>22</v>
       </c>
       <c r="S15" s="10">
@@ -1602,34 +1916,42 @@
         <f>-23+36</f>
         <v>13</v>
       </c>
-      <c r="AD15" s="3">
+      <c r="V15" s="2">
+        <f>-19+37</f>
+        <v>18</v>
+      </c>
+      <c r="AI15" s="3">
         <v>-121</v>
       </c>
-      <c r="AE15" s="3">
+      <c r="AJ15" s="3">
         <v>-121</v>
       </c>
-      <c r="AF15" s="3">
+      <c r="AK15" s="3">
         <f>-94-165</f>
         <v>-259</v>
       </c>
-      <c r="AG15" s="3">
+      <c r="AL15" s="3">
         <f>-47-47</f>
         <v>-94</v>
       </c>
-      <c r="AH15" s="3">
+      <c r="AM15" s="3">
         <f>-34+55</f>
         <v>21</v>
       </c>
-      <c r="AI15" s="3">
+      <c r="AN15" s="3">
         <f>-88+8</f>
         <v>-80</v>
       </c>
-      <c r="AJ15">
+      <c r="AO15">
         <f>-106+197</f>
         <v>91</v>
       </c>
-    </row>
-    <row r="16" spans="1:45" x14ac:dyDescent="0.2">
+      <c r="AP15" s="13">
+        <f t="shared" ref="AP15" si="15">SUM(S15:V15)</f>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="16" spans="1:50" x14ac:dyDescent="0.2">
       <c r="B16" t="s">
         <v>32</v>
       </c>
@@ -1647,67 +1969,75 @@
         <v>948</v>
       </c>
       <c r="N16" s="10">
-        <f t="shared" ref="N16" si="10">N14+N15</f>
+        <f t="shared" ref="N16" si="16">N14+N15</f>
         <v>890</v>
       </c>
       <c r="O16" s="10">
-        <f t="shared" ref="O16:U16" si="11">O14+O15</f>
+        <f t="shared" ref="O16:U16" si="17">O14+O15</f>
         <v>686</v>
       </c>
       <c r="P16" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>683</v>
       </c>
       <c r="Q16" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>907</v>
       </c>
       <c r="R16" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>993</v>
       </c>
       <c r="S16" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>673</v>
       </c>
       <c r="T16" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>892</v>
       </c>
       <c r="U16" s="10">
-        <f t="shared" si="11"/>
+        <f t="shared" si="17"/>
         <v>1308</v>
       </c>
-      <c r="AD16" s="3">
-        <f t="shared" ref="AD16:AJ16" si="12">+AD14+AD15</f>
+      <c r="V16" s="10">
+        <f t="shared" ref="V16" si="18">V14+V15</f>
+        <v>1648</v>
+      </c>
+      <c r="AI16" s="3">
+        <f t="shared" ref="AI16:AP16" si="19">+AI14+AI15</f>
         <v>30</v>
       </c>
-      <c r="AE16" s="3">
-        <f t="shared" si="12"/>
+      <c r="AJ16" s="3">
+        <f t="shared" si="19"/>
         <v>330</v>
       </c>
-      <c r="AF16" s="3">
-        <f t="shared" si="12"/>
+      <c r="AK16" s="3">
+        <f t="shared" si="19"/>
         <v>312</v>
       </c>
-      <c r="AG16" s="3">
-        <f t="shared" si="12"/>
+      <c r="AL16" s="3">
+        <f t="shared" si="19"/>
         <v>1275</v>
       </c>
-      <c r="AH16" s="3">
-        <f t="shared" si="12"/>
+      <c r="AM16" s="3">
+        <f t="shared" si="19"/>
         <v>3657</v>
       </c>
-      <c r="AI16" s="3">
-        <f t="shared" si="12"/>
+      <c r="AN16" s="3">
+        <f t="shared" si="19"/>
         <v>4630</v>
       </c>
-      <c r="AJ16" s="3">
-        <f t="shared" si="12"/>
+      <c r="AO16" s="3">
+        <f t="shared" si="19"/>
         <v>3269</v>
       </c>
-    </row>
-    <row r="17" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AP16" s="3">
+        <f t="shared" si="19"/>
+        <v>4521</v>
+      </c>
+    </row>
+    <row r="17" spans="2:42" x14ac:dyDescent="0.2">
       <c r="B17" t="s">
         <v>33</v>
       </c>
@@ -1732,7 +2062,7 @@
         <v>-39</v>
       </c>
       <c r="R17" s="10">
-        <f>+AJ17-Q17-P17-O17</f>
+        <f>+AO17-Q17-P17-O17</f>
         <v>395</v>
       </c>
       <c r="S17" s="10">
@@ -1744,31 +2074,38 @@
       <c r="U17" s="2">
         <v>-27</v>
       </c>
-      <c r="AD17" s="3">
+      <c r="V17" s="2">
+        <v>419</v>
+      </c>
+      <c r="AI17" s="3">
         <f>9+2</f>
         <v>11</v>
       </c>
-      <c r="AE17" s="3">
+      <c r="AJ17" s="3">
         <f>9+2</f>
         <v>11</v>
       </c>
-      <c r="AF17" s="3">
+      <c r="AK17" s="3">
         <v>0</v>
       </c>
-      <c r="AG17" s="3">
+      <c r="AL17" s="3">
         <v>0</v>
       </c>
-      <c r="AH17" s="3">
+      <c r="AM17" s="3">
         <v>513</v>
       </c>
-      <c r="AI17" s="3">
+      <c r="AN17" s="3">
         <v>0</v>
       </c>
-      <c r="AJ17" s="3">
+      <c r="AO17" s="3">
         <v>346</v>
       </c>
-    </row>
-    <row r="18" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AP17" s="13">
+        <f t="shared" ref="AP17" si="20">SUM(S17:V17)</f>
+        <v>485</v>
+      </c>
+    </row>
+    <row r="18" spans="2:42" x14ac:dyDescent="0.2">
       <c r="B18" t="s">
         <v>34</v>
       </c>
@@ -1786,145 +2123,161 @@
         <v>935</v>
       </c>
       <c r="N18" s="10">
-        <f t="shared" ref="N18" si="13">N16-N17</f>
+        <f t="shared" ref="N18" si="21">N16-N17</f>
         <v>890</v>
       </c>
       <c r="O18" s="10">
-        <f t="shared" ref="O18:U18" si="14">O16-O17</f>
+        <f t="shared" ref="O18:U18" si="22">O16-O17</f>
         <v>673</v>
       </c>
       <c r="P18" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>706</v>
       </c>
       <c r="Q18" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>946</v>
       </c>
       <c r="R18" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>598</v>
       </c>
       <c r="S18" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>621</v>
       </c>
       <c r="T18" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>851</v>
       </c>
       <c r="U18" s="10">
-        <f t="shared" si="14"/>
+        <f t="shared" si="22"/>
         <v>1335</v>
       </c>
-      <c r="AD18" s="3">
-        <f t="shared" ref="AD18:AJ18" si="15">+AD16-AD17</f>
+      <c r="V18" s="10">
+        <f t="shared" ref="V18" si="23">V16-V17</f>
+        <v>1229</v>
+      </c>
+      <c r="AI18" s="3">
+        <f t="shared" ref="AI18:AP18" si="24">+AI16-AI17</f>
         <v>19</v>
       </c>
-      <c r="AE18" s="3">
-        <f t="shared" si="15"/>
+      <c r="AJ18" s="3">
+        <f t="shared" si="24"/>
         <v>319</v>
       </c>
-      <c r="AF18" s="3">
-        <f t="shared" si="15"/>
+      <c r="AK18" s="3">
+        <f t="shared" si="24"/>
         <v>312</v>
       </c>
-      <c r="AG18" s="3">
-        <f t="shared" si="15"/>
+      <c r="AL18" s="3">
+        <f t="shared" si="24"/>
         <v>1275</v>
       </c>
-      <c r="AH18" s="3">
-        <f t="shared" si="15"/>
+      <c r="AM18" s="3">
+        <f t="shared" si="24"/>
         <v>3144</v>
       </c>
-      <c r="AI18" s="3">
-        <f t="shared" si="15"/>
+      <c r="AN18" s="3">
+        <f t="shared" si="24"/>
         <v>4630</v>
       </c>
-      <c r="AJ18" s="3">
-        <f t="shared" si="15"/>
+      <c r="AO18" s="3">
+        <f t="shared" si="24"/>
         <v>2923</v>
       </c>
-    </row>
-    <row r="19" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AP18" s="3">
+        <f t="shared" si="24"/>
+        <v>4036</v>
+      </c>
+    </row>
+    <row r="19" spans="2:42" x14ac:dyDescent="0.2">
       <c r="B19" t="s">
         <v>24</v>
       </c>
       <c r="J19" s="11"/>
       <c r="K19" s="11">
-        <f t="shared" ref="K19:U19" si="16">K18/K20</f>
+        <f t="shared" ref="K19:U19" si="25">K18/K20</f>
         <v>0.83617021276595749</v>
       </c>
       <c r="L19" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>0.89460784313725494</v>
       </c>
       <c r="M19" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>0.58038485412787089</v>
       </c>
       <c r="N19" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>0.56651814131126665</v>
       </c>
       <c r="O19" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>0.41775294847920547</v>
       </c>
       <c r="P19" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>0.4339274738783036</v>
       </c>
       <c r="Q19" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>0.58072437077961936</v>
       </c>
       <c r="R19" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>0.36799999999999999</v>
       </c>
       <c r="S19" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>0.37888956680902991</v>
       </c>
       <c r="T19" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>0.51985339034819789</v>
       </c>
       <c r="U19" s="11">
-        <f t="shared" si="16"/>
+        <f t="shared" si="25"/>
         <v>0.81601466992665039</v>
       </c>
-      <c r="AD19" s="1">
-        <f t="shared" ref="AD19:AJ19" si="17">+AD18/AD20</f>
+      <c r="V19" s="11">
+        <f t="shared" ref="V19" si="26">V18/V20</f>
+        <v>0.75214198286413714</v>
+      </c>
+      <c r="AI19" s="1">
+        <f t="shared" ref="AI19:AP19" si="27">+AI18/AI20</f>
         <v>1.9957983193277309E-2</v>
       </c>
-      <c r="AE19" s="1">
-        <f t="shared" si="17"/>
+      <c r="AJ19" s="1">
+        <f t="shared" si="27"/>
         <v>0.29981203007518797</v>
       </c>
-      <c r="AF19" s="1">
-        <f t="shared" si="17"/>
+      <c r="AK19" s="1">
+        <f t="shared" si="27"/>
         <v>0.27857142857142858</v>
       </c>
-      <c r="AG19" s="1">
-        <f t="shared" si="17"/>
+      <c r="AL19" s="1">
+        <f t="shared" si="27"/>
         <v>1.056338028169014</v>
       </c>
-      <c r="AH19" s="1">
-        <f t="shared" si="17"/>
+      <c r="AM19" s="1">
+        <f t="shared" si="27"/>
         <v>2.5581773799837264</v>
       </c>
-      <c r="AI19" s="1">
-        <f t="shared" si="17"/>
+      <c r="AN19" s="1">
+        <f t="shared" si="27"/>
         <v>2.9471674092934435</v>
       </c>
-      <c r="AJ19" s="1">
-        <f t="shared" si="17"/>
+      <c r="AO19" s="1">
+        <f t="shared" si="27"/>
         <v>1.7987692307692307</v>
       </c>
-    </row>
-    <row r="20" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AP19" s="1">
+        <f t="shared" si="27"/>
+        <v>2.4662389245340668</v>
+      </c>
+    </row>
+    <row r="20" spans="2:42" x14ac:dyDescent="0.2">
       <c r="B20" t="s">
         <v>1</v>
       </c>
@@ -1939,7 +2292,7 @@
         <v>1611</v>
       </c>
       <c r="N20" s="10">
-        <f>+AI20</f>
+        <f>+AN20</f>
         <v>1571</v>
       </c>
       <c r="O20" s="10">
@@ -1952,7 +2305,7 @@
         <v>1629</v>
       </c>
       <c r="R20" s="10">
-        <f>+AJ20</f>
+        <f>+AO20</f>
         <v>1625</v>
       </c>
       <c r="S20" s="10">
@@ -1964,29 +2317,36 @@
       <c r="U20" s="10">
         <v>1636</v>
       </c>
-      <c r="AD20" s="3">
+      <c r="V20" s="10">
+        <v>1634</v>
+      </c>
+      <c r="AI20" s="3">
         <v>952</v>
       </c>
-      <c r="AE20" s="3">
+      <c r="AJ20" s="3">
         <v>1064</v>
       </c>
-      <c r="AF20" s="3">
+      <c r="AK20" s="3">
         <v>1120</v>
       </c>
-      <c r="AG20" s="3">
+      <c r="AL20" s="3">
         <v>1207</v>
       </c>
-      <c r="AH20" s="3">
+      <c r="AM20" s="3">
         <v>1229</v>
       </c>
-      <c r="AI20" s="3">
+      <c r="AN20" s="3">
         <v>1571</v>
       </c>
-      <c r="AJ20" s="3">
+      <c r="AO20" s="3">
         <v>1625</v>
       </c>
-    </row>
-    <row r="23" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AP20" s="3">
+        <f>AVERAGE(S20:V20)</f>
+        <v>1636.5</v>
+      </c>
+    </row>
+    <row r="23" spans="2:42" x14ac:dyDescent="0.2">
       <c r="B23" t="s">
         <v>35</v>
       </c>
@@ -1996,71 +2356,83 @@
         <v>-9.0708340411075228E-2</v>
       </c>
       <c r="P23" s="12">
-        <f t="shared" ref="P23:U23" si="18">P8/L8-1</f>
+        <f t="shared" ref="P23:W23" si="28">P8/L8-1</f>
         <v>-0.18183206106870231</v>
       </c>
       <c r="Q23" s="12">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>4.2228212039532753E-2</v>
       </c>
       <c r="R23" s="12">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>0.10162529023039824</v>
       </c>
       <c r="S23" s="12">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>2.2417336073230043E-2</v>
       </c>
       <c r="T23" s="12">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>8.882254151894009E-2</v>
       </c>
       <c r="U23" s="12">
-        <f t="shared" si="18"/>
+        <f t="shared" si="28"/>
         <v>0.17568965517241386</v>
       </c>
-      <c r="AA23" s="7">
-        <f t="shared" ref="AA23:AD23" si="19">+AA8/Z8-1</f>
+      <c r="V23" s="12">
+        <f t="shared" si="28"/>
+        <v>0.24156939040207526</v>
+      </c>
+      <c r="W23" s="12">
+        <f t="shared" si="28"/>
+        <v>0.29727754430842324</v>
+      </c>
+      <c r="AF23" s="7">
+        <f t="shared" ref="AF23:AI23" si="29">+AF8/AE8-1</f>
         <v>3.9063974334780038E-2</v>
       </c>
-      <c r="AB23" s="7">
-        <f t="shared" si="19"/>
+      <c r="AG23" s="7">
+        <f t="shared" si="29"/>
         <v>-0.27515437704322554</v>
       </c>
-      <c r="AC23" s="7">
-        <f t="shared" si="19"/>
+      <c r="AH23" s="7">
+        <f t="shared" si="29"/>
         <v>7.0408418942620843E-2</v>
       </c>
-      <c r="AD23" s="7">
-        <f t="shared" si="19"/>
+      <c r="AI23" s="7">
+        <f t="shared" si="29"/>
         <v>0.24742509363295873</v>
       </c>
-      <c r="AE23" s="7">
-        <f t="shared" ref="AE23:AJ23" si="20">+AE8/AD8-1</f>
+      <c r="AJ23" s="7">
+        <f t="shared" ref="AJ23:AP23" si="30">+AJ8/AI8-1</f>
         <v>0.21504972790392185</v>
       </c>
-      <c r="AF23" s="7">
-        <f t="shared" si="20"/>
+      <c r="AK23" s="7">
+        <f t="shared" si="30"/>
         <v>3.9536679536679609E-2</v>
       </c>
-      <c r="AG23" s="7">
-        <f t="shared" si="20"/>
+      <c r="AL23" s="7">
+        <f t="shared" si="30"/>
         <v>0.45045312732134901</v>
       </c>
-      <c r="AH23" s="7">
-        <f t="shared" si="20"/>
+      <c r="AM23" s="7">
+        <f t="shared" si="30"/>
         <v>0.68329406944586712</v>
       </c>
-      <c r="AI23" s="7">
-        <f t="shared" si="20"/>
+      <c r="AN23" s="7">
+        <f t="shared" si="30"/>
         <v>0.43610806863818907</v>
       </c>
-      <c r="AJ23" s="7">
-        <f t="shared" si="20"/>
+      <c r="AO23" s="7">
+        <f t="shared" si="30"/>
         <v>-3.9023770179229644E-2</v>
       </c>
-    </row>
-    <row r="25" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AP23" s="7">
+        <f>+AP8/AO8-1</f>
+        <v>0.13690476190476186</v>
+      </c>
+    </row>
+    <row r="25" spans="2:42" x14ac:dyDescent="0.2">
       <c r="B25" t="s">
         <v>26</v>
       </c>
@@ -2074,11 +2446,11 @@
         <v>0.52442748091603053</v>
       </c>
       <c r="M25" s="12">
-        <f t="shared" ref="M25:N25" si="21">M10/M8</f>
+        <f t="shared" ref="M25:N25" si="31">M10/M8</f>
         <v>0.49703504043126684</v>
       </c>
       <c r="N25" s="12">
-        <f t="shared" si="21"/>
+        <f t="shared" si="31"/>
         <v>0.5083050544740132</v>
       </c>
       <c r="O25" s="12">
@@ -2086,59 +2458,84 @@
         <v>0.49766486082570521</v>
       </c>
       <c r="P25" s="12">
-        <f t="shared" ref="P25:U25" si="22">P10/P8</f>
+        <f t="shared" ref="P25:W25" si="32">P10/P8</f>
         <v>0.49542825153946629</v>
       </c>
       <c r="Q25" s="12">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v>0.5098275862068965</v>
       </c>
       <c r="R25" s="12">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v>0.50680933852140075</v>
       </c>
       <c r="S25" s="12">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v>0.5097752603690846</v>
       </c>
       <c r="T25" s="12">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v>0.53041988003427587</v>
       </c>
       <c r="U25" s="12">
-        <f t="shared" si="22"/>
+        <f t="shared" si="32"/>
         <v>0.53556239917876525</v>
       </c>
-      <c r="AD25" s="7">
-        <f>+AD10/AD8</f>
+      <c r="V25" s="12">
+        <f t="shared" si="32"/>
+        <v>0.53982763123530952</v>
+      </c>
+      <c r="W25" s="12">
+        <f t="shared" si="32"/>
+        <v>0</v>
+      </c>
+      <c r="AI25" s="7">
+        <f>+AI10/AI8</f>
         <v>0.3495965471945956</v>
       </c>
-      <c r="AE25" s="7">
-        <f>+AE10/AE8</f>
+      <c r="AJ25" s="7">
+        <f>+AJ10/AJ8</f>
         <v>0.37791505791505792</v>
       </c>
-      <c r="AF25" s="7">
-        <f>+AF10/AF8</f>
+      <c r="AK25" s="7">
+        <f>+AK10/AK8</f>
         <v>0.42608824840291187</v>
       </c>
-      <c r="AG25" s="7">
-        <f t="shared" ref="AG25:AJ25" si="23">+AG10/AG8</f>
+      <c r="AL25" s="7">
+        <f t="shared" ref="AL25:AP25" si="33">+AL10/AL8</f>
         <v>0.44525248386766364</v>
       </c>
-      <c r="AH25" s="7">
-        <f t="shared" si="23"/>
+      <c r="AM25" s="7">
+        <f t="shared" si="33"/>
         <v>0.48247535596933189</v>
       </c>
-      <c r="AI25" s="7">
-        <f t="shared" si="23"/>
+      <c r="AN25" s="7">
+        <f t="shared" si="33"/>
         <v>0.51061395703571888</v>
       </c>
-      <c r="AJ25" s="7">
-        <f t="shared" si="23"/>
+      <c r="AO25" s="7">
+        <f t="shared" si="33"/>
         <v>0.5027336860670194</v>
       </c>
-    </row>
-    <row r="29" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="AP25" s="7">
+        <f t="shared" si="33"/>
+        <v>0.53019197207678881</v>
+      </c>
+    </row>
+    <row r="28" spans="2:42" x14ac:dyDescent="0.2">
+      <c r="B28" t="s">
+        <v>67</v>
+      </c>
+      <c r="U28" s="10">
+        <f>+U29-U45</f>
+        <v>4681</v>
+      </c>
+      <c r="V28" s="10">
+        <f>+V29-V45</f>
+        <v>3560</v>
+      </c>
+    </row>
+    <row r="29" spans="2:42" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
         <v>3</v>
       </c>
@@ -2146,56 +2543,78 @@
         <f>3897+647+137</f>
         <v>4681</v>
       </c>
-    </row>
-    <row r="30" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="V29" s="10">
+        <f>3787+1345+149</f>
+        <v>5281</v>
+      </c>
+    </row>
+    <row r="30" spans="2:42" x14ac:dyDescent="0.2">
       <c r="B30" t="s">
         <v>46</v>
       </c>
       <c r="U30" s="10">
         <v>7241</v>
       </c>
-    </row>
-    <row r="31" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="V30" s="10">
+        <v>6192</v>
+      </c>
+    </row>
+    <row r="31" spans="2:42" x14ac:dyDescent="0.2">
       <c r="B31" t="s">
         <v>47</v>
       </c>
       <c r="U31" s="10">
         <v>5374</v>
       </c>
-    </row>
-    <row r="32" spans="2:36" x14ac:dyDescent="0.2">
+      <c r="V31" s="10">
+        <v>5734</v>
+      </c>
+    </row>
+    <row r="32" spans="2:42" x14ac:dyDescent="0.2">
       <c r="B32" t="s">
         <v>48</v>
       </c>
       <c r="U32" s="10">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="V32" s="10">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="33" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B33" t="s">
         <v>49</v>
       </c>
       <c r="U33" s="10">
         <v>1547</v>
       </c>
-    </row>
-    <row r="34" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="V33" s="10">
+        <v>1878</v>
+      </c>
+    </row>
+    <row r="34" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B34" t="s">
         <v>50</v>
       </c>
       <c r="U34" s="10">
         <v>1669</v>
       </c>
-    </row>
-    <row r="35" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="V34" s="10">
+        <v>1802</v>
+      </c>
+    </row>
+    <row r="35" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B35" t="s">
         <v>51</v>
       </c>
       <c r="U35" s="10">
         <v>647</v>
       </c>
-    </row>
-    <row r="36" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="V35" s="10">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="36" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B36" t="s">
         <v>44</v>
       </c>
@@ -2203,24 +2622,34 @@
         <f>24839+19572</f>
         <v>44411</v>
       </c>
-    </row>
-    <row r="37" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="V36" s="10">
+        <f>24839+18930</f>
+        <v>43769</v>
+      </c>
+    </row>
+    <row r="37" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B37" t="s">
         <v>45</v>
       </c>
       <c r="U37" s="10">
         <v>1183</v>
       </c>
-    </row>
-    <row r="38" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="V37" s="10">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="38" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B38" t="s">
         <v>53</v>
       </c>
       <c r="U38" s="10">
         <v>2854</v>
       </c>
-    </row>
-    <row r="39" spans="2:23" x14ac:dyDescent="0.2">
+      <c r="V38" s="10">
+        <v>3146</v>
+      </c>
+    </row>
+    <row r="39" spans="2:28" x14ac:dyDescent="0.2">
       <c r="B39" t="s">
         <v>52</v>
       </c>
@@ -2228,8 +2657,15 @@
         <f>SUM(U29:U38)</f>
         <v>69636</v>
       </c>
-    </row>
-    <row r="41" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="V39" s="10">
+        <f>SUM(V29:V38)</f>
+        <v>69226</v>
+      </c>
+    </row>
+    <row r="41" spans="2:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="C41" s="10"/>
       <c r="D41" s="10"/>
       <c r="E41" s="10"/>
@@ -2248,13 +2684,21 @@
       <c r="R41" s="10"/>
       <c r="S41" s="10"/>
       <c r="T41" s="10"/>
-      <c r="U41" s="10">
-        <v>2530</v>
-      </c>
-      <c r="V41" s="10"/>
+      <c r="U41" s="10"/>
+      <c r="V41" s="10">
+        <v>1990</v>
+      </c>
       <c r="W41" s="10"/>
-    </row>
-    <row r="42" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X41" s="10"/>
+      <c r="Y41" s="10"/>
+      <c r="Z41" s="10"/>
+      <c r="AA41" s="10"/>
+      <c r="AB41" s="10"/>
+    </row>
+    <row r="42" spans="2:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B42" s="3" t="s">
+        <v>65</v>
+      </c>
       <c r="C42" s="10"/>
       <c r="D42" s="10"/>
       <c r="E42" s="10"/>
@@ -2273,13 +2717,21 @@
       <c r="R42" s="10"/>
       <c r="S42" s="10"/>
       <c r="T42" s="10"/>
-      <c r="U42" s="10">
-        <v>461</v>
-      </c>
-      <c r="V42" s="10"/>
+      <c r="U42" s="10"/>
+      <c r="V42" s="10">
+        <v>476</v>
+      </c>
       <c r="W42" s="10"/>
-    </row>
-    <row r="43" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X42" s="10"/>
+      <c r="Y42" s="10"/>
+      <c r="Z42" s="10"/>
+      <c r="AA42" s="10"/>
+      <c r="AB42" s="10"/>
+    </row>
+    <row r="43" spans="2:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B43" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="C43" s="10"/>
       <c r="D43" s="10"/>
       <c r="E43" s="10"/>
@@ -2298,13 +2750,21 @@
       <c r="R43" s="10"/>
       <c r="S43" s="10"/>
       <c r="T43" s="10"/>
-      <c r="U43" s="10">
-        <v>4120</v>
-      </c>
-      <c r="V43" s="10"/>
+      <c r="U43" s="10"/>
+      <c r="V43" s="10">
+        <v>4260</v>
+      </c>
       <c r="W43" s="10"/>
-    </row>
-    <row r="44" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X43" s="10"/>
+      <c r="Y43" s="10"/>
+      <c r="Z43" s="10"/>
+      <c r="AA43" s="10"/>
+      <c r="AB43" s="10"/>
+    </row>
+    <row r="44" spans="2:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B44" s="3" t="s">
+        <v>63</v>
+      </c>
       <c r="C44" s="10"/>
       <c r="D44" s="10"/>
       <c r="E44" s="10"/>
@@ -2323,13 +2783,21 @@
       <c r="R44" s="10"/>
       <c r="S44" s="10"/>
       <c r="T44" s="10"/>
-      <c r="U44" s="10">
-        <v>389</v>
-      </c>
-      <c r="V44" s="10"/>
+      <c r="U44" s="10"/>
+      <c r="V44" s="10">
+        <v>555</v>
+      </c>
       <c r="W44" s="10"/>
-    </row>
-    <row r="45" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X44" s="10"/>
+      <c r="Y44" s="10"/>
+      <c r="Z44" s="10"/>
+      <c r="AA44" s="10"/>
+      <c r="AB44" s="10"/>
+    </row>
+    <row r="45" spans="2:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="3" t="s">
+        <v>4</v>
+      </c>
       <c r="C45" s="10"/>
       <c r="D45" s="10"/>
       <c r="E45" s="10"/>
@@ -2349,10 +2817,20 @@
       <c r="S45" s="10"/>
       <c r="T45" s="10"/>
       <c r="U45" s="10"/>
-      <c r="V45" s="10"/>
+      <c r="V45" s="10">
+        <v>1721</v>
+      </c>
       <c r="W45" s="10"/>
-    </row>
-    <row r="46" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X45" s="10"/>
+      <c r="Y45" s="10"/>
+      <c r="Z45" s="10"/>
+      <c r="AA45" s="10"/>
+      <c r="AB45" s="10"/>
+    </row>
+    <row r="46" spans="2:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="3" t="s">
+        <v>62</v>
+      </c>
       <c r="C46" s="10"/>
       <c r="D46" s="10"/>
       <c r="E46" s="10"/>
@@ -2372,10 +2850,20 @@
       <c r="S46" s="10"/>
       <c r="T46" s="10"/>
       <c r="U46" s="10"/>
-      <c r="V46" s="10"/>
+      <c r="V46" s="10">
+        <v>491</v>
+      </c>
       <c r="W46" s="10"/>
-    </row>
-    <row r="47" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X46" s="10"/>
+      <c r="Y46" s="10"/>
+      <c r="Z46" s="10"/>
+      <c r="AA46" s="10"/>
+      <c r="AB46" s="10"/>
+    </row>
+    <row r="47" spans="2:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B47" s="3" t="s">
+        <v>61</v>
+      </c>
       <c r="C47" s="10"/>
       <c r="D47" s="10"/>
       <c r="E47" s="10"/>
@@ -2395,10 +2883,20 @@
       <c r="S47" s="10"/>
       <c r="T47" s="10"/>
       <c r="U47" s="10"/>
-      <c r="V47" s="10"/>
+      <c r="V47" s="10">
+        <v>349</v>
+      </c>
       <c r="W47" s="10"/>
-    </row>
-    <row r="48" spans="2:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X47" s="10"/>
+      <c r="Y47" s="10"/>
+      <c r="Z47" s="10"/>
+      <c r="AA47" s="10"/>
+      <c r="AB47" s="10"/>
+    </row>
+    <row r="48" spans="2:28" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B48" s="3" t="s">
+        <v>60</v>
+      </c>
       <c r="C48" s="10"/>
       <c r="D48" s="10"/>
       <c r="E48" s="10"/>
@@ -2418,10 +2916,20 @@
       <c r="S48" s="10"/>
       <c r="T48" s="10"/>
       <c r="U48" s="10"/>
-      <c r="V48" s="10"/>
+      <c r="V48" s="10">
+        <v>1816</v>
+      </c>
       <c r="W48" s="10"/>
-    </row>
-    <row r="49" spans="3:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X48" s="10"/>
+      <c r="Y48" s="10"/>
+      <c r="Z48" s="10"/>
+      <c r="AA48" s="10"/>
+      <c r="AB48" s="10"/>
+    </row>
+    <row r="49" spans="2:42" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="3" t="s">
+        <v>59</v>
+      </c>
       <c r="C49" s="10"/>
       <c r="D49" s="10"/>
       <c r="E49" s="10"/>
@@ -2441,10 +2949,20 @@
       <c r="S49" s="10"/>
       <c r="T49" s="10"/>
       <c r="U49" s="10"/>
-      <c r="V49" s="10"/>
+      <c r="V49" s="10">
+        <v>57568</v>
+      </c>
       <c r="W49" s="10"/>
-    </row>
-    <row r="50" spans="3:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X49" s="10"/>
+      <c r="Y49" s="10"/>
+      <c r="Z49" s="10"/>
+      <c r="AA49" s="10"/>
+      <c r="AB49" s="10"/>
+    </row>
+    <row r="50" spans="2:42" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="3" t="s">
+        <v>58</v>
+      </c>
       <c r="C50" s="10"/>
       <c r="D50" s="10"/>
       <c r="E50" s="10"/>
@@ -2464,10 +2982,18 @@
       <c r="S50" s="10"/>
       <c r="T50" s="10"/>
       <c r="U50" s="10"/>
-      <c r="V50" s="10"/>
+      <c r="V50" s="10">
+        <f>SUM(V41:V49)</f>
+        <v>69226</v>
+      </c>
       <c r="W50" s="10"/>
-    </row>
-    <row r="51" spans="3:23" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="X50" s="10"/>
+      <c r="Y50" s="10"/>
+      <c r="Z50" s="10"/>
+      <c r="AA50" s="10"/>
+      <c r="AB50" s="10"/>
+    </row>
+    <row r="51" spans="2:42" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="C51" s="10"/>
       <c r="D51" s="10"/>
       <c r="E51" s="10"/>
@@ -2489,6 +3015,174 @@
       <c r="U51" s="10"/>
       <c r="V51" s="10"/>
       <c r="W51" s="10"/>
+      <c r="X51" s="10"/>
+      <c r="Y51" s="10"/>
+      <c r="Z51" s="10"/>
+      <c r="AA51" s="10"/>
+      <c r="AB51" s="10"/>
+    </row>
+    <row r="52" spans="2:42" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B52" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
+      <c r="F52" s="10"/>
+      <c r="G52" s="10"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="10"/>
+      <c r="J52" s="10"/>
+      <c r="K52" s="10"/>
+      <c r="L52" s="10"/>
+      <c r="M52" s="10"/>
+      <c r="N52" s="10"/>
+      <c r="O52" s="10"/>
+      <c r="P52" s="10"/>
+      <c r="Q52" s="10"/>
+      <c r="R52" s="10"/>
+      <c r="S52" s="10"/>
+      <c r="T52" s="10"/>
+      <c r="U52" s="10"/>
+      <c r="V52" s="10"/>
+      <c r="W52" s="10"/>
+      <c r="X52" s="10"/>
+      <c r="Y52" s="10"/>
+      <c r="Z52" s="10"/>
+      <c r="AA52" s="10"/>
+      <c r="AB52" s="10"/>
+      <c r="AJ52" s="3">
+        <v>34</v>
+      </c>
+      <c r="AK52" s="3">
+        <v>493</v>
+      </c>
+      <c r="AL52" s="3">
+        <v>1071</v>
+      </c>
+      <c r="AM52" s="3">
+        <v>3521</v>
+      </c>
+      <c r="AN52" s="3">
+        <v>3565</v>
+      </c>
+      <c r="AO52" s="3">
+        <v>1667</v>
+      </c>
+      <c r="AP52" s="3">
+        <v>3041</v>
+      </c>
+    </row>
+    <row r="53" spans="2:42" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B53" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C53" s="10"/>
+      <c r="D53" s="10"/>
+      <c r="E53" s="10"/>
+      <c r="F53" s="10"/>
+      <c r="G53" s="10"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="10"/>
+      <c r="J53" s="10"/>
+      <c r="K53" s="10"/>
+      <c r="L53" s="10"/>
+      <c r="M53" s="10"/>
+      <c r="N53" s="10"/>
+      <c r="O53" s="10"/>
+      <c r="P53" s="10"/>
+      <c r="Q53" s="10"/>
+      <c r="R53" s="10"/>
+      <c r="S53" s="10"/>
+      <c r="T53" s="10"/>
+      <c r="U53" s="10"/>
+      <c r="V53" s="10"/>
+      <c r="W53" s="10"/>
+      <c r="X53" s="10"/>
+      <c r="Y53" s="10"/>
+      <c r="Z53" s="10"/>
+      <c r="AA53" s="10"/>
+      <c r="AB53" s="10"/>
+      <c r="AJ53" s="3">
+        <v>163</v>
+      </c>
+      <c r="AK53" s="3">
+        <v>149</v>
+      </c>
+      <c r="AL53" s="3">
+        <v>294</v>
+      </c>
+      <c r="AM53" s="3">
+        <v>301</v>
+      </c>
+      <c r="AN53" s="3">
+        <v>450</v>
+      </c>
+      <c r="AO53" s="3">
+        <v>546</v>
+      </c>
+      <c r="AP53" s="3">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="54" spans="2:42" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C54" s="10"/>
+      <c r="D54" s="10"/>
+      <c r="E54" s="10"/>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="10"/>
+      <c r="K54" s="10"/>
+      <c r="L54" s="10"/>
+      <c r="M54" s="10"/>
+      <c r="N54" s="10"/>
+      <c r="O54" s="10"/>
+      <c r="P54" s="10"/>
+      <c r="Q54" s="10"/>
+      <c r="R54" s="10"/>
+      <c r="S54" s="10"/>
+      <c r="T54" s="10"/>
+      <c r="U54" s="10"/>
+      <c r="V54" s="10"/>
+      <c r="W54" s="10"/>
+      <c r="X54" s="10"/>
+      <c r="Y54" s="10"/>
+      <c r="Z54" s="10"/>
+      <c r="AA54" s="10"/>
+      <c r="AB54" s="10"/>
+      <c r="AJ54" s="3">
+        <f t="shared" ref="AJ54:AN54" si="34">+AJ52-AJ53</f>
+        <v>-129</v>
+      </c>
+      <c r="AK54" s="3">
+        <f t="shared" si="34"/>
+        <v>344</v>
+      </c>
+      <c r="AL54" s="3">
+        <f t="shared" si="34"/>
+        <v>777</v>
+      </c>
+      <c r="AM54" s="3">
+        <f t="shared" si="34"/>
+        <v>3220</v>
+      </c>
+      <c r="AN54" s="3">
+        <f t="shared" si="34"/>
+        <v>3115</v>
+      </c>
+      <c r="AO54" s="3">
+        <f>+AO52-AO53</f>
+        <v>1121</v>
+      </c>
+      <c r="AP54" s="3">
+        <f>+AP52-AP53</f>
+        <v>2405</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>